<commit_message>
Pushing an updated log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Cardiac Output" sheetId="13" r:id="rId9"/>
     <sheet name="Blood Volume" sheetId="12" r:id="rId10"/>
     <sheet name="Calories Used" sheetId="2" r:id="rId11"/>
+    <sheet name="Insulin Receptors" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
@@ -151,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="162">
   <si>
     <t>Bone</t>
   </si>
@@ -589,6 +590,54 @@
   </si>
   <si>
     <t>BV (mL)</t>
+  </si>
+  <si>
+    <t>Insulin Receptors (Units are mU, mU/mL and mU/Min)</t>
+  </si>
+  <si>
+    <t>Non-Hepatic Mass</t>
+  </si>
+  <si>
+    <t>Hepatic Receptors (/kG BW)</t>
+  </si>
+  <si>
+    <t>Non-Hepatic Receptors (/kG BW)</t>
+  </si>
+  <si>
+    <t>Total (mU)</t>
+  </si>
+  <si>
+    <t>Secretion=Degradation (mU/Min)</t>
+  </si>
+  <si>
+    <t>[Insulin] ECFV</t>
+  </si>
+  <si>
+    <t>% Occupied</t>
+  </si>
+  <si>
+    <t>Degradation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>% Total</t>
+  </si>
+  <si>
+    <t>Occupied</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>mU/Min</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>[Insulin] Portal Vein</t>
   </si>
 </sst>
 </file>
@@ -1598,12 +1647,340 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3">
+        <f>BodyMassMale</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <f>BoneMassMale</f>
+        <v>10725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <f>BrainMassMale</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <f>GIMassMale</f>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <f>KidneyMassMale</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <f>LHeartMassMale</f>
+        <v>292.57499999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <f>LiverMassMale</f>
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <f>OtherMassMale</f>
+        <v>3525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <f>RMuscleMassMale</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <f>RHeartMassMale</f>
+        <v>59.924999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1">
+        <f>SkinMassMale</f>
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <f>SUM(B6:B17)</f>
+        <v>68482.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="1">
+        <f>SUM(B6:B11,B13:B17)</f>
+        <v>66532.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22">
+        <v>204</v>
+      </c>
+      <c r="C22">
+        <f>BodyMassMale*B22</f>
+        <v>15300</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <f>0.01*D22*C22</f>
+        <v>1836</v>
+      </c>
+      <c r="F22">
+        <f>C22-E22</f>
+        <v>13464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23">
+        <v>183</v>
+      </c>
+      <c r="C23">
+        <f>BodyMassMale*B23</f>
+        <v>13725</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <f>0.01*D23*C23</f>
+        <v>274.5</v>
+      </c>
+      <c r="F23">
+        <f>C23-E23</f>
+        <v>13450.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27">
+        <v>0.02</v>
+      </c>
+      <c r="C27">
+        <v>15000</v>
+      </c>
+      <c r="D27">
+        <f>B27*C27</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>79</v>
+      </c>
+      <c r="C31">
+        <f>0.01*B31*B25</f>
+        <v>13.43</v>
+      </c>
+      <c r="D31">
+        <f>C31/E22</f>
+        <v>7.3148148148148148E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <f>0.01*B32*B25</f>
+        <v>1.53</v>
+      </c>
+      <c r="D32">
+        <f>C32/D27</f>
+        <v>5.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <f>0.01*B33*B25</f>
+        <v>2.04</v>
+      </c>
+      <c r="D33">
+        <f>C33/E23</f>
+        <v>7.4316939890710382E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f>SUM(C31:C33)</f>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,7 +3567,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A3" sqref="A3:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4661,7 +5038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Pushing a current log and also a current normal values Excel spreadsheet.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="168">
   <si>
     <t>Bone</t>
   </si>
@@ -595,15 +595,6 @@
     <t>Insulin Receptors (Units are mU, mU/mL and mU/Min)</t>
   </si>
   <si>
-    <t>Non-Hepatic Mass</t>
-  </si>
-  <si>
-    <t>Hepatic Receptors (/kG BW)</t>
-  </si>
-  <si>
-    <t>Non-Hepatic Receptors (/kG BW)</t>
-  </si>
-  <si>
     <t>Total (mU)</t>
   </si>
   <si>
@@ -613,31 +604,58 @@
     <t>[Insulin] ECFV</t>
   </si>
   <si>
-    <t>% Occupied</t>
-  </si>
-  <si>
     <t>Degradation</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>% Total</t>
   </si>
   <si>
-    <t>Occupied</t>
-  </si>
-  <si>
     <t>Free</t>
   </si>
   <si>
     <t>mU/Min</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
     <t>[Insulin] Portal Vein</t>
+  </si>
+  <si>
+    <t>Binding = K1 * [I] * Free - K2 * Bound</t>
+  </si>
+  <si>
+    <t>K1 = 10 * K2</t>
+  </si>
+  <si>
+    <t>General and Liver Degradation = K3 * Bound</t>
+  </si>
+  <si>
+    <t>Kidney Degradation = K4 * [I] * GFR</t>
+  </si>
+  <si>
+    <t>[I] = Pool for General and Kidney and Portal for Liver</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>K3 and K4</t>
+  </si>
+  <si>
+    <t>% Bound</t>
+  </si>
+  <si>
+    <t>Bound</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Hepatic Receptors (mU)</t>
+  </si>
+  <si>
+    <t>General Receptors (mU)</t>
   </si>
 </sst>
 </file>
@@ -1649,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,14 +1679,15 @@
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -1677,301 +1696,214 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1">
-        <f>BoneMassMale</f>
-        <v>10725</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <f>BrainMassMale</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <f>FatMassMale</f>
-        <v>16050</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <f>GIMassMale</f>
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1">
-        <f>KidneyMassMale</f>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
-        <f>LHeartMassMale</f>
-        <v>292.57499999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1">
-        <f>LiverMassMale</f>
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C12">
+        <v>50000</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <f>0.01*D12*C12</f>
+        <v>10000</v>
+      </c>
+      <c r="F12">
+        <f>C12-E12</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1">
-        <f>OtherMassMale</f>
-        <v>3525</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13">
+        <v>19000</v>
+      </c>
+      <c r="D13">
         <v>8</v>
       </c>
-      <c r="B14" s="1">
-        <f>RMuscleMassMale</f>
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>0.01*D13*C13</f>
+        <v>1520</v>
+      </c>
+      <c r="F13">
+        <f>C13-E13</f>
+        <v>17480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1">
-        <f>RHeartMassMale</f>
-        <v>59.924999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1">
-        <f>SMuscleMassMale</f>
-        <v>26400</v>
+        <v>148</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1">
-        <f>SkinMassMale</f>
-        <v>2775</v>
+        <v>149</v>
+      </c>
+      <c r="B17">
+        <v>0.02</v>
+      </c>
+      <c r="C17">
+        <v>15000</v>
+      </c>
+      <c r="D17">
+        <f>B17*C17</f>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1">
-        <f>SUM(B6:B17)</f>
-        <v>68482.5</v>
+        <v>154</v>
+      </c>
+      <c r="B18">
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="1">
-        <f>SUM(B6:B11,B13:B17)</f>
-        <v>66532.5</v>
+        <v>150</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" t="s">
-        <v>157</v>
-      </c>
-      <c r="F21" t="s">
-        <v>158</v>
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>79</v>
+      </c>
+      <c r="C21">
+        <f>0.01*B21*B15</f>
+        <v>13.43</v>
+      </c>
+      <c r="D21">
+        <f>C21/E12</f>
+        <v>1.343E-3</v>
+      </c>
+      <c r="E21">
+        <f>10*F21</f>
+        <v>1.2435185185185186E-2</v>
+      </c>
+      <c r="F21">
+        <f>C21/(10*B18*F12-E12)</f>
+        <v>1.2435185185185186E-3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>204</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <f>BodyMassMale*B22</f>
-        <v>15300</v>
+        <f>0.01*B22*B15</f>
+        <v>1.53</v>
       </c>
       <c r="D22">
-        <v>12</v>
-      </c>
-      <c r="E22">
-        <f>0.01*D22*C22</f>
-        <v>1836</v>
-      </c>
-      <c r="F22">
-        <f>C22-E22</f>
-        <v>13464</v>
+        <f>C22/(1000*B17*125)</f>
+        <v>6.1200000000000002E-4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B23">
-        <v>183</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <f>BodyMassMale*B23</f>
-        <v>13725</v>
+        <f>0.01*B23*B15</f>
+        <v>2.04</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <f>C23/E13</f>
+        <v>1.3421052631578947E-3</v>
       </c>
       <c r="E23">
-        <f>0.01*D23*C23</f>
-        <v>274.5</v>
+        <f>10*F23</f>
+        <v>1.0323886639676113E-2</v>
       </c>
       <c r="F23">
-        <f>C23-E23</f>
-        <v>13450.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B25">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27">
-        <v>0.02</v>
-      </c>
-      <c r="C27">
-        <v>15000</v>
-      </c>
-      <c r="D27">
-        <f>B27*C27</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28">
-        <v>5.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <v>79</v>
-      </c>
-      <c r="C31">
-        <f>0.01*B31*B25</f>
-        <v>13.43</v>
-      </c>
-      <c r="D31">
-        <f>C31/E22</f>
-        <v>7.3148148148148148E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32">
-        <v>9</v>
-      </c>
-      <c r="C32">
-        <f>0.01*B32*B25</f>
-        <v>1.53</v>
-      </c>
-      <c r="D32">
-        <f>C32/D27</f>
-        <v>5.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B33">
-        <v>12</v>
-      </c>
-      <c r="C33">
-        <f>0.01*B33*B25</f>
-        <v>2.04</v>
-      </c>
-      <c r="D33">
-        <f>C33/E23</f>
-        <v>7.4316939890710382E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <f>SUM(C31:C33)</f>
+        <f>C23/(10*B17*F13-E13)</f>
+        <v>1.0323886639676113E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f>SUM(C21:C23)</f>
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2012-10-24. HumModRepository edits. Smaller 'Log' cloud button on home page. Spreadsheets listed and linked on 'Normal Values' home page. Data | CO2 Transport describes a submodel for calculating [HCO3] as a function of pCO2 and [SID].
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Blood Volume" sheetId="12" r:id="rId10"/>
     <sheet name="Calories Used" sheetId="2" r:id="rId11"/>
     <sheet name="Insulin Receptors" sheetId="14" r:id="rId12"/>
+    <sheet name="PV-Arteries" sheetId="15" r:id="rId13"/>
+    <sheet name="PV-Veins" sheetId="16" r:id="rId14"/>
+    <sheet name="PV-Lungs" sheetId="17" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
@@ -33,6 +36,10 @@
     <definedName name="BaseMassFemale">'Organ Mass - Female'!$D$16</definedName>
     <definedName name="BaseMassMale">'Organ Mass - Male'!$C$16</definedName>
     <definedName name="BloodMass">'Organ Mass - Male'!$C$19</definedName>
+    <definedName name="BloodVolume_Male">'Blood Volume'!$D$12</definedName>
+    <definedName name="BloodVolume_Male_Arteries">'PV-Arteries'!$B$4</definedName>
+    <definedName name="BloodVolume_Male_Lungs">'PV-Arteries'!$D$4</definedName>
+    <definedName name="BloodVolume_Male_Veins">'PV-Arteries'!$C$4</definedName>
     <definedName name="BodyMassFemale">'Body Mass'!$B$5</definedName>
     <definedName name="BodyMassMale">'Body Mass'!$B$4</definedName>
     <definedName name="BoneFlowFemale">'Organ Blood Flow'!$H$11</definedName>
@@ -47,6 +54,7 @@
     <definedName name="CardiacOutputMale">'Organ Blood Flow'!$D$4</definedName>
     <definedName name="CoronaryGradient">'Pressure Gradients'!$D$6</definedName>
     <definedName name="CoronarySinusOutflow">'Flows &amp; Conductances'!$B$30</definedName>
+    <definedName name="Density">'PV-Arteries'!$G$3</definedName>
     <definedName name="EfferentArtyGradient">'Pressure Gradients'!$D$9</definedName>
     <definedName name="FatFlowFemale">'Organ Blood Flow'!$H$9</definedName>
     <definedName name="FatFlowGFemale">'Organ Blood Flow'!$J$9</definedName>
@@ -92,6 +100,7 @@
     <definedName name="LungH2OMass">'Organ Mass - Male'!$C$20</definedName>
     <definedName name="LungMassFemale">'Organ Mass - Female'!$D$33</definedName>
     <definedName name="LungMassMale">'Organ Mass - Male'!$C$39</definedName>
+    <definedName name="Male_Height">'PV-Arteries'!$E$3</definedName>
     <definedName name="MuscleFlowFemale">'Organ Blood Flow'!$H$19</definedName>
     <definedName name="MuscleFlowMale">'Organ Blood Flow'!$C$19</definedName>
     <definedName name="MuscleMassFemale">'Organ Mass - Female'!$C$25</definedName>
@@ -148,11 +157,12 @@
     <definedName name="VenousReturn">'Flows &amp; Conductances'!$B$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="212">
   <si>
     <t>Bone</t>
   </si>
@@ -656,6 +666,138 @@
   </si>
   <si>
     <t>General Receptors (mU)</t>
+  </si>
+  <si>
+    <t>Cerebral</t>
+  </si>
+  <si>
+    <t>Carotid</t>
+  </si>
+  <si>
+    <t>BloodVolume</t>
+  </si>
+  <si>
+    <t>~~~ ARTERY ~~~</t>
+  </si>
+  <si>
+    <t>Thoracic Aorta</t>
+  </si>
+  <si>
+    <t>Abdominal Aorta</t>
+  </si>
+  <si>
+    <t>Right Iliac</t>
+  </si>
+  <si>
+    <t>Left Iliac</t>
+  </si>
+  <si>
+    <t>~~~ SUMS ~~~</t>
+  </si>
+  <si>
+    <t>F-BV</t>
+  </si>
+  <si>
+    <t>F-Height</t>
+  </si>
+  <si>
+    <t>F-Arteries</t>
+  </si>
+  <si>
+    <t>F-Veins</t>
+  </si>
+  <si>
+    <t>F-Lungs</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>~~~ VEINS ~~~</t>
+  </si>
+  <si>
+    <t>Jugular</t>
+  </si>
+  <si>
+    <t>Superior VenaCava</t>
+  </si>
+  <si>
+    <t>Right Ventricle</t>
+  </si>
+  <si>
+    <t>Inferior VenaCava</t>
+  </si>
+  <si>
+    <t>Splanchnic</t>
+  </si>
+  <si>
+    <t>~~~ SUMS</t>
+  </si>
+  <si>
+    <t>Male-Veins</t>
+  </si>
+  <si>
+    <t>Male-Lungs</t>
+  </si>
+  <si>
+    <t>~~~ LUNGS ~~~</t>
+  </si>
+  <si>
+    <t>Left Ventricle</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Ortho-P</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>P-Ext</t>
+  </si>
+  <si>
+    <t>F-V0</t>
+  </si>
+  <si>
+    <t>V0</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>Right LowerArm</t>
+  </si>
+  <si>
+    <t>Right UpperArm</t>
+  </si>
+  <si>
+    <t>Left UpperArm</t>
+  </si>
+  <si>
+    <t>Left LowerArm</t>
+  </si>
+  <si>
+    <t>Right Thigh</t>
+  </si>
+  <si>
+    <t>Right Calf</t>
+  </si>
+  <si>
+    <t>Right Foot</t>
+  </si>
+  <si>
+    <t>Left Thigh</t>
+  </si>
+  <si>
+    <t>Left Calf</t>
+  </si>
+  <si>
+    <t>Left Foot</t>
   </si>
 </sst>
 </file>
@@ -704,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -720,6 +862,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,7 +1238,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1904,6 +2058,2200 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>SUM(B3:D3)</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.18</v>
+      </c>
+      <c r="C3">
+        <v>0.67</v>
+      </c>
+      <c r="D3">
+        <v>0.15</v>
+      </c>
+      <c r="E3">
+        <v>178</v>
+      </c>
+      <c r="F3">
+        <v>0.7</v>
+      </c>
+      <c r="G3">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>BloodVolume_Male</f>
+        <v>5407.95</v>
+      </c>
+      <c r="B4" s="1">
+        <f>B3*A4</f>
+        <v>973.43099999999993</v>
+      </c>
+      <c r="C4" s="1">
+        <f>C3*A4</f>
+        <v>3623.3265000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <f>D3*A4</f>
+        <v>811.1925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" ref="C6:C21" si="0">B6*BloodVolume_Male_Arteries</f>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" ref="E6:E21" si="1">D6*Male_Height</f>
+        <v>169.1</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" ref="F6:F21" si="2">(Male_Height-E6)*Density</f>
+        <v>11.926000000000009</v>
+      </c>
+      <c r="G6" s="12">
+        <f>F6-F7</f>
+        <v>-19.081600000000012</v>
+      </c>
+      <c r="H6" s="11">
+        <v>95</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" ref="J6:J21" si="3">H6-I6</f>
+        <v>95</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L6" s="12">
+        <f t="shared" ref="L6:L21" si="4">K6*C6</f>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" ref="M6:M21" si="5">(C6-L6)/J6</f>
+        <v>7.6849815789473711E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.87</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="1"/>
+        <v>154.85999999999999</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="2"/>
+        <v>31.007600000000021</v>
+      </c>
+      <c r="G7" s="12">
+        <f>F7-F12</f>
+        <v>-16.696399999999972</v>
+      </c>
+      <c r="H7" s="11">
+        <v>97</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L7" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="5"/>
+        <v>7.5265283505154656E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="1"/>
+        <v>142.4</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
+        <v>47.703999999999994</v>
+      </c>
+      <c r="G8" s="12">
+        <f>F8-F10</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>95</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="5"/>
+        <v>7.6849815789473711E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="C9" s="12">
+        <f t="shared" si="0"/>
+        <v>58.40585999999999</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="1"/>
+        <v>124.6</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="2"/>
+        <v>71.556000000000012</v>
+      </c>
+      <c r="G9" s="12">
+        <f>F9-F8</f>
+        <v>23.852000000000018</v>
+      </c>
+      <c r="H9" s="11">
+        <v>93</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L9" s="12">
+        <f t="shared" si="4"/>
+        <v>49.644980999999987</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="5"/>
+        <v>9.4203000000000023E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="1"/>
+        <v>142.4</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="2"/>
+        <v>47.703999999999994</v>
+      </c>
+      <c r="G10" s="12">
+        <f>F10-F12</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>95</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L10" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="5"/>
+        <v>7.6849815789473711E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="0"/>
+        <v>58.40585999999999</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="E11" s="12">
+        <f t="shared" si="1"/>
+        <v>124.6</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="2"/>
+        <v>71.556000000000012</v>
+      </c>
+      <c r="G11" s="12">
+        <f>F11-F10</f>
+        <v>23.852000000000018</v>
+      </c>
+      <c r="H11" s="11">
+        <v>93</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L11" s="12">
+        <f t="shared" si="4"/>
+        <v>49.644980999999987</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="5"/>
+        <v>9.4203000000000023E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="0"/>
+        <v>146.01464999999999</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="1"/>
+        <v>142.4</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="2"/>
+        <v>47.703999999999994</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>97</v>
+      </c>
+      <c r="I12" s="11">
+        <v>-3</v>
+      </c>
+      <c r="J12" s="13">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L12" s="12">
+        <f t="shared" si="4"/>
+        <v>124.11245249999999</v>
+      </c>
+      <c r="M12" s="14">
+        <f t="shared" si="5"/>
+        <v>0.21902197500000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0.17</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="0"/>
+        <v>165.48327</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.65</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="1"/>
+        <v>115.7</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="2"/>
+        <v>83.481999999999999</v>
+      </c>
+      <c r="G13" s="12">
+        <f>F13-F12</f>
+        <v>35.778000000000006</v>
+      </c>
+      <c r="H13" s="11">
+        <v>97</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L13" s="12">
+        <f t="shared" si="4"/>
+        <v>140.66077949999999</v>
+      </c>
+      <c r="M13" s="14">
+        <f t="shared" si="5"/>
+        <v>0.25590196391752595</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="2"/>
+        <v>119.26</v>
+      </c>
+      <c r="G14" s="12">
+        <f>F14-F13</f>
+        <v>35.778000000000006</v>
+      </c>
+      <c r="H14" s="11">
+        <v>95</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L14" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="5"/>
+        <v>7.6849815789473711E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="0"/>
+        <v>58.40585999999999</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.37</v>
+      </c>
+      <c r="E15" s="12">
+        <f t="shared" si="1"/>
+        <v>65.86</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="2"/>
+        <v>150.26760000000002</v>
+      </c>
+      <c r="G15" s="12">
+        <f>F15-F14</f>
+        <v>31.007600000000011</v>
+      </c>
+      <c r="H15" s="11">
+        <v>94</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L15" s="12">
+        <f t="shared" si="4"/>
+        <v>49.644980999999987</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" si="5"/>
+        <v>9.320084042553195E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="12">
+        <f t="shared" si="1"/>
+        <v>35.6</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="2"/>
+        <v>190.81600000000003</v>
+      </c>
+      <c r="G16" s="12">
+        <f>F16-F15</f>
+        <v>40.548400000000015</v>
+      </c>
+      <c r="H16" s="11">
+        <v>92</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L16" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="5"/>
+        <v>7.9355788043478287E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="0"/>
+        <v>19.468619999999998</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="E17" s="12">
+        <f t="shared" si="1"/>
+        <v>3.56</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="2"/>
+        <v>233.74960000000002</v>
+      </c>
+      <c r="G17" s="12">
+        <f>F17-F16</f>
+        <v>42.933599999999984</v>
+      </c>
+      <c r="H17" s="11">
+        <v>89</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L17" s="12">
+        <f t="shared" si="4"/>
+        <v>16.548326999999997</v>
+      </c>
+      <c r="M17" s="14">
+        <f t="shared" si="5"/>
+        <v>3.2812280898876417E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="12">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="2"/>
+        <v>119.26</v>
+      </c>
+      <c r="G18" s="12">
+        <f>F18-F13</f>
+        <v>35.778000000000006</v>
+      </c>
+      <c r="H18" s="11">
+        <v>95</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L18" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M18" s="14">
+        <f t="shared" si="5"/>
+        <v>7.6849815789473711E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="0"/>
+        <v>58.40585999999999</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.37</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="1"/>
+        <v>65.86</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="2"/>
+        <v>150.26760000000002</v>
+      </c>
+      <c r="G19" s="12">
+        <f>F19-F18</f>
+        <v>31.007600000000011</v>
+      </c>
+      <c r="H19" s="11">
+        <v>94</v>
+      </c>
+      <c r="I19" s="11">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L19" s="12">
+        <f t="shared" si="4"/>
+        <v>49.644980999999987</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="5"/>
+        <v>9.320084042553195E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="0"/>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="12">
+        <f t="shared" si="1"/>
+        <v>35.6</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="2"/>
+        <v>190.81600000000003</v>
+      </c>
+      <c r="G20" s="12">
+        <f>F20-F19</f>
+        <v>40.548400000000015</v>
+      </c>
+      <c r="H20" s="11">
+        <v>92</v>
+      </c>
+      <c r="I20" s="11">
+        <v>0</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L20" s="12">
+        <f t="shared" si="4"/>
+        <v>41.370817499999994</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="5"/>
+        <v>7.9355788043478287E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="0"/>
+        <v>19.468619999999998</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="1"/>
+        <v>3.56</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="2"/>
+        <v>233.74960000000002</v>
+      </c>
+      <c r="G21" s="12">
+        <f>F21-F20</f>
+        <v>42.933599999999984</v>
+      </c>
+      <c r="H21" s="11">
+        <v>89</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="L21" s="12">
+        <f t="shared" si="4"/>
+        <v>16.548326999999997</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="5"/>
+        <v>3.2812280898876417E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="11">
+        <f>SUM(B6:B21)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C22" s="12">
+        <f>SUM(C6:C21)</f>
+        <v>973.43100000000004</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12">
+        <f>SUM(L6:L21)</f>
+        <v>827.41635000000008</v>
+      </c>
+      <c r="M22" s="14">
+        <f>SUM(M6:M21)</f>
+        <v>1.5335821201058228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <f>BloodVolume_Male_Veins</f>
+        <v>3623.3265000000001</v>
+      </c>
+      <c r="E2">
+        <f>Male_Height</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6">
+        <v>0.04</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C24" si="0">B6*BloodVolume_Male_Veins</f>
+        <v>144.93306000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6:E24" si="1">D6*Male_Height</f>
+        <v>169.1</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F24" si="2">(Male_Height-E6)*Density</f>
+        <v>11.926000000000009</v>
+      </c>
+      <c r="G6" s="5">
+        <f>F6-F7</f>
+        <v>-19.081600000000012</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6:J24" si="3">H6-I6</f>
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>0.95</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" ref="L6:L24" si="4">K6*C6</f>
+        <v>137.686407</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" ref="M6:M24" si="5">(C6-L6)/J6</f>
+        <v>0.90583162500000114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>72.466530000000006</v>
+      </c>
+      <c r="D7">
+        <v>0.87</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>154.85999999999999</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="2"/>
+        <v>31.007600000000021</v>
+      </c>
+      <c r="G7" s="5">
+        <f>F7-F12</f>
+        <v>-26.237199999999984</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" si="4"/>
+        <v>36.233265000000003</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="5"/>
+        <v>5.1761807142857146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8">
+        <v>0.03</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D8">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>142.4</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="2"/>
+        <v>47.703999999999994</v>
+      </c>
+      <c r="G8" s="5">
+        <f>F8-F12</f>
+        <v>-9.5408000000000115</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>0.6</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" si="4"/>
+        <v>65.219876999999997</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="5"/>
+        <v>5.4349897499999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9">
+        <v>0.02</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>72.466530000000006</v>
+      </c>
+      <c r="D9">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>124.6</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="2"/>
+        <v>71.556000000000012</v>
+      </c>
+      <c r="G9" s="5">
+        <f>F9-F8</f>
+        <v>23.852000000000018</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>0.7</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="4"/>
+        <v>50.726571</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="5"/>
+        <v>2.1739959000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10">
+        <v>0.03</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>142.4</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="2"/>
+        <v>47.703999999999994</v>
+      </c>
+      <c r="G10" s="5">
+        <f>F10-F12</f>
+        <v>-9.5408000000000115</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0.6</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" si="4"/>
+        <v>65.219876999999997</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" si="5"/>
+        <v>5.4349897499999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11">
+        <v>0.02</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>72.466530000000006</v>
+      </c>
+      <c r="D11">
+        <v>0.7</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>124.6</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="2"/>
+        <v>71.556000000000012</v>
+      </c>
+      <c r="G11" s="5">
+        <f>F11-F10</f>
+        <v>23.852000000000018</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>0.7</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="4"/>
+        <v>50.726571</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" si="5"/>
+        <v>2.1739959000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12">
+        <v>0.12</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>434.79917999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.76</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>135.28</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="2"/>
+        <v>57.244800000000005</v>
+      </c>
+      <c r="G12" s="5">
+        <f>F12-F13</f>
+        <v>-9.5407999999999973</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>-3</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>0.3</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="4"/>
+        <v>130.43975399999999</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" si="5"/>
+        <v>33.817713999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>0.02</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>72.466530000000006</v>
+      </c>
+      <c r="D13">
+        <v>0.72</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>128.16</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="2"/>
+        <v>66.785600000000002</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>-3</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="5"/>
+        <v>10.352361428571429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14">
+        <v>0.03</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D14">
+        <v>0.72</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>128.16</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="2"/>
+        <v>66.785600000000002</v>
+      </c>
+      <c r="G14" s="5">
+        <f>F14-F13</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>-3</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="5"/>
+        <v>15.528542142857143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15">
+        <v>0.24</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>869.59835999999996</v>
+      </c>
+      <c r="D15">
+        <v>0.65</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>115.7</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="2"/>
+        <v>83.481999999999999</v>
+      </c>
+      <c r="G15" s="5">
+        <f>F15-F13</f>
+        <v>16.696399999999997</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>0.3</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="4"/>
+        <v>260.87950799999999</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="5"/>
+        <v>60.871885199999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16">
+        <v>0.25</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>905.83162500000003</v>
+      </c>
+      <c r="D16">
+        <v>0.68</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>121.04</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="2"/>
+        <v>76.326399999999992</v>
+      </c>
+      <c r="G16" s="5">
+        <f>F16-F13</f>
+        <v>9.5407999999999902</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" si="4"/>
+        <v>452.91581250000002</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" si="5"/>
+        <v>90.5831625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17">
+        <v>0.03</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="2"/>
+        <v>119.26</v>
+      </c>
+      <c r="G17" s="5">
+        <f>F17-F15</f>
+        <v>35.778000000000006</v>
+      </c>
+      <c r="H17">
+        <v>12</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <v>0.6</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="4"/>
+        <v>65.219876999999997</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="5"/>
+        <v>3.6233264999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18">
+        <v>0.03</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D18">
+        <v>0.37</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>65.86</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="2"/>
+        <v>150.26760000000002</v>
+      </c>
+      <c r="G18" s="5">
+        <f>F18-F17</f>
+        <v>31.007600000000011</v>
+      </c>
+      <c r="H18">
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="K18">
+        <v>0.7</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="4"/>
+        <v>76.089856499999996</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="5"/>
+        <v>2.3292813214285712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19">
+        <v>0.02</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="0"/>
+        <v>72.466530000000006</v>
+      </c>
+      <c r="D19">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>35.6</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="2"/>
+        <v>190.81600000000003</v>
+      </c>
+      <c r="G19" s="5">
+        <f>F19-F18</f>
+        <v>40.548400000000015</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="K19">
+        <v>0.8</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="4"/>
+        <v>57.973224000000009</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="5"/>
+        <v>0.85254741176470572</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20">
+        <v>0.01</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="0"/>
+        <v>36.233265000000003</v>
+      </c>
+      <c r="D20">
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>3.56</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="2"/>
+        <v>233.74960000000002</v>
+      </c>
+      <c r="G20" s="5">
+        <f>F20-F19</f>
+        <v>42.933599999999984</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>0.9</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" si="4"/>
+        <v>32.609938500000005</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" si="5"/>
+        <v>0.18116632499999988</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21">
+        <v>0.03</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="2"/>
+        <v>119.26</v>
+      </c>
+      <c r="G21" s="5">
+        <f>F21-F15</f>
+        <v>35.778000000000006</v>
+      </c>
+      <c r="H21">
+        <v>12</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>0.6</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" si="4"/>
+        <v>65.219876999999997</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" si="5"/>
+        <v>3.6233264999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22">
+        <v>0.03</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="0"/>
+        <v>108.69979499999999</v>
+      </c>
+      <c r="D22">
+        <v>0.37</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>65.86</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="2"/>
+        <v>150.26760000000002</v>
+      </c>
+      <c r="G22" s="5">
+        <f>F22-F21</f>
+        <v>31.007600000000011</v>
+      </c>
+      <c r="H22">
+        <v>14</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="K22">
+        <v>0.7</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="4"/>
+        <v>76.089856499999996</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="5"/>
+        <v>2.3292813214285712</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23">
+        <v>0.02</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="0"/>
+        <v>72.466530000000006</v>
+      </c>
+      <c r="D23">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>35.6</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="2"/>
+        <v>190.81600000000003</v>
+      </c>
+      <c r="G23" s="5">
+        <f>F23-F22</f>
+        <v>40.548400000000015</v>
+      </c>
+      <c r="H23">
+        <v>17</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="K23">
+        <v>0.8</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="4"/>
+        <v>57.973224000000009</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="5"/>
+        <v>0.85254741176470572</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24">
+        <v>0.01</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="0"/>
+        <v>36.233265000000003</v>
+      </c>
+      <c r="D24">
+        <v>0.02</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>3.56</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="2"/>
+        <v>233.74960000000002</v>
+      </c>
+      <c r="G24" s="5">
+        <f>F24-F23</f>
+        <v>42.933599999999984</v>
+      </c>
+      <c r="H24">
+        <v>20</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K24">
+        <v>0.9</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" si="4"/>
+        <v>32.609938500000005</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="5"/>
+        <v>0.18116632499999988</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25">
+        <f>SUM(B6:B24)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C25" s="1">
+        <f>SUM(C6:C24)</f>
+        <v>3623.3265000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <f>BloodVolume_Male_Lungs</f>
+        <v>811.1925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.27</v>
+      </c>
+      <c r="C6" s="12">
+        <f>B6*BloodVolume_Male_Lungs</f>
+        <v>219.02197500000003</v>
+      </c>
+      <c r="D6" s="11">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11">
+        <v>-3</v>
+      </c>
+      <c r="F6" s="12">
+        <f>D6-E6</f>
+        <v>18</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="12">
+        <f>G6*C6</f>
+        <v>109.51098750000001</v>
+      </c>
+      <c r="I6" s="12">
+        <f>(C6-H6)/F6</f>
+        <v>6.0839437500000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.27</v>
+      </c>
+      <c r="C7" s="12">
+        <f>B7*BloodVolume_Male_Lungs</f>
+        <v>219.02197500000003</v>
+      </c>
+      <c r="D7" s="11">
+        <v>12</v>
+      </c>
+      <c r="E7" s="11">
+        <v>-3</v>
+      </c>
+      <c r="F7" s="12">
+        <f>D7-E7</f>
+        <v>15</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="H7" s="12">
+        <f>G7*C7</f>
+        <v>153.3153825</v>
+      </c>
+      <c r="I7" s="12">
+        <f>(C7-H7)/F7</f>
+        <v>4.3804395000000023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C8" s="12">
+        <f>B8*BloodVolume_Male_Lungs</f>
+        <v>235.245825</v>
+      </c>
+      <c r="D8" s="11">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11">
+        <v>-3</v>
+      </c>
+      <c r="F8" s="12">
+        <f>D8-E8</f>
+        <v>12</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="12">
+        <f>G8*C8</f>
+        <v>164.6720775</v>
+      </c>
+      <c r="I8" s="12">
+        <f>(C8-H8)/F8</f>
+        <v>5.8811456249999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="C9" s="12">
+        <f>B9*BloodVolume_Male_Lungs</f>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="D9" s="11">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11">
+        <v>-3</v>
+      </c>
+      <c r="F9" s="12">
+        <f>D9-E9</f>
+        <v>11</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <f>G9*C9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <f>(C9-H9)/F9</f>
+        <v>4.4246863636363631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="C10" s="12">
+        <f>B10*BloodVolume_Male_Lungs</f>
+        <v>89.231174999999993</v>
+      </c>
+      <c r="D10" s="11">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11">
+        <v>-3</v>
+      </c>
+      <c r="F10" s="12">
+        <f>D10-E10</f>
+        <v>11</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <f>G10*C10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <f>(C10-H10)/F10</f>
+        <v>8.1119249999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="11">
+        <f>SUM(B6:B10)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C11" s="13">
+        <f>SUM(C6:C10)</f>
+        <v>811.19250000000011</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4029,7 +6377,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4170,7 +6518,7 @@
         <v>19767.150000000001</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" ref="J9:J13" si="2">H9/I9</f>
+        <f t="shared" ref="J9:J14" si="2">H9/I9</f>
         <v>1.8715596330275232E-2</v>
       </c>
       <c r="L9" s="7">
@@ -4365,7 +6713,7 @@
         <v>281.57752808988755</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" ref="J14" si="4">H14/I14</f>
+        <f t="shared" si="2"/>
         <v>0.77285997031172726</v>
       </c>
       <c r="L14" s="7">
@@ -4428,11 +6776,11 @@
         <v>263.60449438202244</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" ref="J16:J17" si="5">H16/I16</f>
+        <f t="shared" ref="J16:J21" si="4">H16/I16</f>
         <v>2.8068868921775909</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" ref="L16:L21" si="6">(E16+J16)/2</f>
+        <f t="shared" ref="L16:L21" si="5">(E16+J16)/2</f>
         <v>2.9579889006342501</v>
       </c>
     </row>
@@ -4467,11 +6815,11 @@
         <v>1557.6629213483143</v>
       </c>
       <c r="J17" s="7">
+        <f t="shared" si="4"/>
+        <v>0.75443023255813979</v>
+      </c>
+      <c r="L17" s="7">
         <f t="shared" si="5"/>
-        <v>0.75443023255813979</v>
-      </c>
-      <c r="L17" s="7">
-        <f t="shared" si="6"/>
         <v>0.72336896243291604</v>
       </c>
     </row>
@@ -4506,11 +6854,11 @@
         <v>459.42</v>
       </c>
       <c r="J18" s="7">
-        <f>H18/I18</f>
+        <f t="shared" si="4"/>
         <v>0.23684210526315791</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.23684210526315791</v>
       </c>
     </row>
@@ -4545,11 +6893,11 @@
         <v>17504.585393258429</v>
       </c>
       <c r="J19" s="7">
-        <f>H19/I19</f>
+        <f t="shared" si="4"/>
         <v>2.9837210551764894E-2</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3.0218605275882448E-2</v>
       </c>
     </row>
@@ -4584,11 +6932,11 @@
         <v>2216.6741573033705</v>
       </c>
       <c r="J20" s="7">
-        <f>H20/I20</f>
+        <f t="shared" si="4"/>
         <v>9.8174104336895066E-2</v>
       </c>
       <c r="L20" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>9.7735700817096177E-2</v>
       </c>
     </row>
@@ -4623,11 +6971,11 @@
         <v>18.135000000000002</v>
       </c>
       <c r="J21" s="7">
-        <f>H21/I21</f>
+        <f t="shared" si="4"/>
         <v>3.5999999999999996</v>
       </c>
       <c r="L21" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3.5999999999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2012-11-03 HumMod v2.0.38 Pushing a current version of the log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -157,12 +157,47 @@
     <definedName name="VenousReturn">'Flows &amp; Conductances'!$B$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tom Coleman</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Coleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+We can substitute K1 = 10 * K2 and then
+solve for K2 to get
+K2 = NetBinding/(10*[I]* Free - Bound)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="218">
   <si>
     <t>Bone</t>
   </si>
@@ -632,9 +667,6 @@
     <t>Binding = K1 * [I] * Free - K2 * Bound</t>
   </si>
   <si>
-    <t>K1 = 10 * K2</t>
-  </si>
-  <si>
     <t>General and Liver Degradation = K3 * Bound</t>
   </si>
   <si>
@@ -798,6 +830,27 @@
   </si>
   <si>
     <t>Left Foot</t>
+  </si>
+  <si>
+    <t>Hepatic Vein</t>
+  </si>
+  <si>
+    <t>[Insulin]Hepatic</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>Unbinding</t>
+  </si>
+  <si>
+    <t>Net Binding</t>
+  </si>
+  <si>
+    <t>K1 =20 * K2</t>
   </si>
 </sst>
 </file>
@@ -810,7 +863,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,6 +877,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1820,11 +1886,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,25 +1923,25 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="1"/>
     </row>
@@ -1887,10 +1953,10 @@
         <v>147</v>
       </c>
       <c r="D11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" t="s">
         <v>162</v>
-      </c>
-      <c r="E11" t="s">
-        <v>163</v>
       </c>
       <c r="F11" t="s">
         <v>152</v>
@@ -1898,7 +1964,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12">
         <v>50000</v>
@@ -1917,7 +1983,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13">
         <v>19000</v>
@@ -1965,99 +2031,140 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>150</v>
-      </c>
-      <c r="B20" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" t="s">
-        <v>165</v>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>79</v>
-      </c>
-      <c r="C21">
-        <f>0.01*B21*B15</f>
-        <v>13.43</v>
-      </c>
-      <c r="D21">
-        <f>C21/E12</f>
-        <v>1.343E-3</v>
-      </c>
-      <c r="E21">
-        <f>10*F21</f>
-        <v>1.2435185185185186E-2</v>
-      </c>
-      <c r="F21">
-        <f>C21/(10*B18*F12-E12)</f>
-        <v>1.2435185185185186E-3</v>
+        <v>150</v>
+      </c>
+      <c r="B21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="C22">
         <f>0.01*B22*B15</f>
-        <v>1.53</v>
+        <v>13.43</v>
       </c>
       <c r="D22">
-        <f>C22/(1000*B17*125)</f>
-        <v>6.1200000000000002E-4</v>
+        <f>C22/E12</f>
+        <v>1.343E-3</v>
+      </c>
+      <c r="E22">
+        <f>20*F22</f>
+        <v>2.4870370370370373E-2</v>
+      </c>
+      <c r="F22">
+        <f>C22/(20*B19*F12-E12)</f>
+        <v>1.2435185185185186E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <f>0.01*B23*B15</f>
+        <v>1.53</v>
+      </c>
+      <c r="D23">
+        <f>C23/(1000*B17*125)</f>
+        <v>6.1200000000000002E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <f>0.01*B24*B15</f>
         <v>2.04</v>
       </c>
-      <c r="D23">
-        <f>C23/E13</f>
+      <c r="D24">
+        <f>C24/E13</f>
         <v>1.3421052631578947E-3</v>
       </c>
-      <c r="E23">
-        <f>10*F23</f>
+      <c r="E24">
+        <f>10*F24</f>
         <v>1.0323886639676113E-2</v>
       </c>
-      <c r="F23">
-        <f>C23/(10*B17*F13-E13)</f>
+      <c r="F24">
+        <f>C24/(10*B17*F13-E13)</f>
         <v>1.0323886639676113E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <f>SUM(C21:C23)</f>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f>SUM(C22:C24)</f>
         <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28">
+        <f>E22*B19*F12</f>
+        <v>25.865185185185187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29">
+        <f>F22*E12</f>
+        <v>12.435185185185185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30">
+        <f>B28-B29</f>
+        <v>13.430000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2089,25 +2196,25 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
         <v>179</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>180</v>
       </c>
-      <c r="D2" t="s">
-        <v>181</v>
-      </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
         <v>142</v>
       </c>
       <c r="G2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2154,48 +2261,48 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>183</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>200</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="11">
         <v>0.05</v>
@@ -2243,7 +2350,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="11">
         <v>0.05</v>
@@ -2291,7 +2398,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="11">
         <v>0.05</v>
@@ -2339,7 +2446,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" s="11">
         <v>0.06</v>
@@ -2387,7 +2494,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10" s="11">
         <v>0.05</v>
@@ -2435,7 +2542,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="11">
         <v>0.06</v>
@@ -2483,7 +2590,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" s="11">
         <v>0.15</v>
@@ -2530,7 +2637,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="11">
         <v>0.17</v>
@@ -2578,7 +2685,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="11">
         <v>0.05</v>
@@ -2626,7 +2733,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B15" s="11">
         <v>0.06</v>
@@ -2674,7 +2781,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" s="11">
         <v>0.05</v>
@@ -2722,7 +2829,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B17" s="11">
         <v>0.02</v>
@@ -2770,7 +2877,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B18" s="11">
         <v>0.05</v>
@@ -2818,7 +2925,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" s="11">
         <v>0.06</v>
@@ -2866,7 +2973,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="11">
         <v>0.05</v>
@@ -2914,7 +3021,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B21" s="11">
         <v>0.02</v>
@@ -2962,7 +3069,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="11">
         <f>SUM(B6:B21)</f>
@@ -3021,13 +3128,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3042,48 +3149,48 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>183</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>200</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6">
         <v>0.04</v>
@@ -3131,7 +3238,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>0.02</v>
@@ -3179,7 +3286,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8">
         <v>0.03</v>
@@ -3227,7 +3334,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>0.02</v>
@@ -3275,7 +3382,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10">
         <v>0.03</v>
@@ -3323,7 +3430,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <v>0.02</v>
@@ -3371,7 +3478,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B12">
         <v>0.12</v>
@@ -3466,7 +3573,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B14">
         <v>0.03</v>
@@ -3514,7 +3621,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15">
         <v>0.24</v>
@@ -3562,7 +3669,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B16">
         <v>0.25</v>
@@ -3610,7 +3717,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17">
         <v>0.03</v>
@@ -3658,7 +3765,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B18">
         <v>0.03</v>
@@ -3706,7 +3813,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B19">
         <v>0.02</v>
@@ -3754,7 +3861,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20">
         <v>0.01</v>
@@ -3802,7 +3909,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B21">
         <v>0.03</v>
@@ -3850,7 +3957,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B22">
         <v>0.03</v>
@@ -3898,7 +4005,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23">
         <v>0.02</v>
@@ -3946,7 +4053,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B24">
         <v>0.01</v>
@@ -3994,7 +4101,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B25">
         <f>SUM(B6:B24)</f>
@@ -4015,7 +4122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4024,10 +4131,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4038,31 +4145,31 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>78</v>
       </c>
       <c r="G5" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>200</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4199,7 +4306,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="11">
         <v>0.11</v>
@@ -4232,7 +4339,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="11">
         <f>SUM(B6:B10)</f>
@@ -6376,8 +6483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7284,9 +7391,19 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="1"/>
+      <c r="A35" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" s="1">
+        <f>GIFlowMale+HepaticArtyFlowMale</f>
+        <v>1350</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="7"/>
+      <c r="H35">
+        <f>GIFlowFemale+HepaticArtyFlowFemale</f>
+        <v>1175.1480000000001</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
@@ -7318,8 +7435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2013-02-17. Current log. HumMod version bumped to 2.0.50. Finishing up renal O2 shunt and EPO. Added some reference files in Structure to EPO and Kidney-TubuleO2.
EPO now gets 3 panels : pool, secretion and disposal. Added detail includes pG/mL, an [EPO] clamp, parametric volume of distribution and parametric 1/2 life.

RBC's also get 3 panels under Body Fluids | Blood | Red Cells : pool, secretion, disposal. Delay of [EPO] effect on red cell formation and red cell lifespan are now adjustable parameters.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="217">
   <si>
     <t>Bone</t>
   </si>
@@ -490,24 +490,15 @@
     <t>Coronary</t>
   </si>
   <si>
-    <t>Hepatic</t>
-  </si>
-  <si>
     <t>GI Tract (&amp; Hepatic Artery)</t>
   </si>
   <si>
-    <t>Systemic Veins Outflow</t>
-  </si>
-  <si>
     <t>Pulmonary Artery Outflow</t>
   </si>
   <si>
     <t>Pulmonary Capillaries Outflow</t>
   </si>
   <si>
-    <t>Pulmonary Veins Outflow</t>
-  </si>
-  <si>
     <t>Pressures</t>
   </si>
   <si>
@@ -851,6 +842,12 @@
   </si>
   <si>
     <t>K1 =20 * K2</t>
+  </si>
+  <si>
+    <t>Pericardium</t>
+  </si>
+  <si>
+    <t>Splanchnic Vein</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1248,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1304,7 +1301,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,18 +1314,18 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1373,27 +1370,27 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B9" s="1">
         <f>BaseMassMale</f>
@@ -1495,7 +1492,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B13" s="1">
         <f>OrganMassMale</f>
@@ -1537,7 +1534,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1889,7 +1886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -1904,12 +1901,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3">
         <f>BodyMassMale</f>
@@ -1918,30 +1915,30 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B9" s="1"/>
     </row>
@@ -1950,21 +1947,21 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C12">
         <v>50000</v>
@@ -1983,7 +1980,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C13">
         <v>19000</v>
@@ -2002,7 +1999,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B15">
         <v>17</v>
@@ -2010,7 +2007,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B17">
         <v>0.02</v>
@@ -2025,7 +2022,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B18">
         <v>5.1999999999999998E-2</v>
@@ -2033,7 +2030,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B19">
         <v>2.5999999999999999E-2</v>
@@ -2041,22 +2038,22 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" t="s">
         <v>150</v>
       </c>
-      <c r="B21" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" t="s">
-        <v>153</v>
-      </c>
       <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="s">
         <v>160</v>
       </c>
-      <c r="E21" t="s">
-        <v>163</v>
-      </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2101,7 +2098,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -2131,12 +2128,12 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B28">
         <f>E22*B19*F12</f>
@@ -2145,7 +2142,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B29">
         <f>F22*E12</f>
@@ -2154,7 +2151,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B30">
         <f>B28-B29</f>
@@ -2196,25 +2193,25 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" t="s">
         <v>179</v>
       </c>
-      <c r="D2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" t="s">
-        <v>182</v>
-      </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2261,48 +2258,48 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B6" s="11">
         <v>0.05</v>
@@ -2350,7 +2347,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B7" s="11">
         <v>0.05</v>
@@ -2398,7 +2395,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B8" s="11">
         <v>0.05</v>
@@ -2446,7 +2443,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B9" s="11">
         <v>0.06</v>
@@ -2494,7 +2491,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10" s="11">
         <v>0.05</v>
@@ -2542,7 +2539,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B11" s="11">
         <v>0.06</v>
@@ -2590,7 +2587,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B12" s="11">
         <v>0.15</v>
@@ -2637,7 +2634,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B13" s="11">
         <v>0.17</v>
@@ -2685,7 +2682,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B14" s="11">
         <v>0.05</v>
@@ -2733,7 +2730,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B15" s="11">
         <v>0.06</v>
@@ -2781,7 +2778,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B16" s="11">
         <v>0.05</v>
@@ -2829,7 +2826,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B17" s="11">
         <v>0.02</v>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B18" s="11">
         <v>0.05</v>
@@ -2925,7 +2922,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B19" s="11">
         <v>0.06</v>
@@ -2973,7 +2970,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B20" s="11">
         <v>0.05</v>
@@ -3021,7 +3018,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B21" s="11">
         <v>0.02</v>
@@ -3069,7 +3066,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B22" s="11">
         <f>SUM(B6:B21)</f>
@@ -3128,13 +3125,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3149,48 +3146,48 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B6">
         <v>0.04</v>
@@ -3238,7 +3235,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>0.02</v>
@@ -3286,7 +3283,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B8">
         <v>0.03</v>
@@ -3334,7 +3331,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B9">
         <v>0.02</v>
@@ -3382,7 +3379,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10">
         <v>0.03</v>
@@ -3430,7 +3427,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B11">
         <v>0.02</v>
@@ -3478,7 +3475,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B12">
         <v>0.12</v>
@@ -3573,7 +3570,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B14">
         <v>0.03</v>
@@ -3621,7 +3618,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B15">
         <v>0.24</v>
@@ -3669,7 +3666,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B16">
         <v>0.25</v>
@@ -3717,7 +3714,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B17">
         <v>0.03</v>
@@ -3765,7 +3762,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B18">
         <v>0.03</v>
@@ -3813,7 +3810,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B19">
         <v>0.02</v>
@@ -3861,7 +3858,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B20">
         <v>0.01</v>
@@ -3909,7 +3906,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B21">
         <v>0.03</v>
@@ -3957,7 +3954,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B22">
         <v>0.03</v>
@@ -4005,7 +4002,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B23">
         <v>0.02</v>
@@ -4053,7 +4050,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B24">
         <v>0.01</v>
@@ -4101,7 +4098,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B25">
         <f>SUM(B6:B24)</f>
@@ -4131,10 +4128,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4145,31 +4142,31 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>78</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4306,7 +4303,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B10" s="11">
         <v>0.11</v>
@@ -4339,7 +4336,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B11" s="11">
         <f>SUM(B6:B10)</f>
@@ -4654,7 +4651,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B22" s="5">
         <v>1.3</v>
@@ -4666,7 +4663,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B23">
         <v>8.6999999999999993</v>
@@ -4681,7 +4678,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B25" s="5">
         <f>B17+B23</f>
@@ -5304,10 +5301,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5362,7 +5359,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7">
         <f>SystemicArtysPressure-2</f>
@@ -5379,7 +5376,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B8">
         <v>60</v>
@@ -5395,7 +5392,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B9">
         <f>SystemicArtysPressure-3.5</f>
@@ -5412,7 +5409,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B10">
         <f>SystemicArtysPressure-3.5</f>
@@ -5467,15 +5464,15 @@
         <v>70</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="0"/>
-        <v>0.2666</v>
+        <v>0.53320000000000001</v>
       </c>
       <c r="D14">
-        <f>B14-B28</f>
-        <v>6</v>
+        <f>B14-B29</f>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5515,15 +5512,15 @@
         <v>73</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="0"/>
-        <v>0.93310000000000004</v>
+        <v>1.1997</v>
       </c>
       <c r="D17">
         <f>B17-B28</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5531,15 +5528,15 @@
         <v>74</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" si="0"/>
-        <v>0.79980000000000007</v>
+        <v>1.0664</v>
       </c>
       <c r="D18">
-        <f>B18-B28</f>
-        <v>10</v>
+        <f>B18-B29</f>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5637,6 +5634,18 @@
       <c r="C28" s="5">
         <f>0.1333*B28</f>
         <v>-0.53320000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29">
+        <v>-3</v>
+      </c>
+      <c r="C29" s="5">
+        <f>0.1333*B29</f>
+        <v>-0.39990000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -5650,7 +5659,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5659,6 +5668,8 @@
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5668,10 +5679,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5679,10 +5690,10 @@
         <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
         <v>95</v>
@@ -5707,7 +5718,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5">
         <f>SystemicArtysPressure</f>
@@ -5732,16 +5743,16 @@
       </c>
       <c r="C6">
         <f>RightAtrialPressure</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B7">
         <f>SystemicArtysPressure</f>
@@ -5758,7 +5769,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B8">
         <f>ArcuateArtyPressure</f>
@@ -5775,7 +5786,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B9">
         <f>GlomularPressure</f>
@@ -5792,7 +5803,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B10">
         <f>SystemicArtysPressure</f>
@@ -5809,7 +5820,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B11">
         <f>LHeartLargeVesselPressure</f>
@@ -5817,16 +5828,16 @@
       </c>
       <c r="C11">
         <f>RightAtrialPressure</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>89.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B12">
         <f>SystemicArtysPressure</f>
@@ -5843,7 +5854,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B13">
         <f>RHeartLargeVesselPressure</f>
@@ -5851,16 +5862,16 @@
       </c>
       <c r="C13">
         <f>RightAtrialPressure</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>89.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>216</v>
       </c>
       <c r="B14">
         <f>SplanchnicVeinsPressure</f>
@@ -5868,16 +5879,16 @@
       </c>
       <c r="C14">
         <f>RightAtrialPressure</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B15">
         <f>SystemicVeinsPressure</f>
@@ -5885,16 +5896,16 @@
       </c>
       <c r="C15">
         <f>RightAtrialPressure</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B17">
         <f>PulmArtyPressure</f>
@@ -5911,7 +5922,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B18">
         <f>PulmCapysPressure</f>
@@ -5919,24 +5930,24 @@
       </c>
       <c r="C18">
         <f>PulmVeinsPressure</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B19">
         <f>PulmVeinsPressure</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <f>LeftAtrialPressure</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -5971,30 +5982,30 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6023,7 +6034,7 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6383,7 +6394,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>0.44</v>
@@ -6501,7 +6512,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6509,13 +6520,13 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6567,31 +6578,31 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I8" t="s">
         <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -7392,7 +7403,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C35" s="1">
         <f>GIFlowMale+HepaticArtyFlowMale</f>
@@ -7436,7 +7447,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7449,7 +7460,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7457,7 +7468,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
         <v>95</v>
@@ -7466,7 +7477,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
@@ -7631,7 +7642,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B12" s="1">
         <f>OtherFlowMale</f>
@@ -7731,7 +7742,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B16" s="1">
         <f>SUM(B5:B15)</f>
@@ -7739,11 +7750,11 @@
       </c>
       <c r="C16">
         <f>SystemicVeinsGradient</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>479.25</v>
+        <v>639</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
@@ -7810,11 +7821,11 @@
       </c>
       <c r="C20">
         <f>HepaticGradient</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <f>B20/C20</f>
-        <v>225</v>
+        <v>337.5</v>
       </c>
       <c r="E20" s="1">
         <f>LiverMassMale</f>
@@ -7822,7 +7833,7 @@
       </c>
       <c r="F20" s="4">
         <f>D20/E20</f>
-        <v>0.11538461538461539</v>
+        <v>0.17307692307692307</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -7832,7 +7843,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B22" s="1">
         <f>LiverFlowMale</f>
@@ -7840,11 +7851,11 @@
       </c>
       <c r="C22">
         <f>HepaticGradient</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <f>B22/C22</f>
-        <v>225</v>
+        <v>337.5</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="4"/>
@@ -7864,11 +7875,11 @@
       </c>
       <c r="C24">
         <f>CoronaryGradient</f>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D24" s="6">
         <f>B24/C24</f>
-        <v>1.8871578947368421</v>
+        <v>1.927741935483871</v>
       </c>
       <c r="E24" s="1">
         <f>LHeartMassMale</f>
@@ -7876,7 +7887,7 @@
       </c>
       <c r="F24" s="4">
         <f>D24/E24</f>
-        <v>6.4501679731243013E-3</v>
+        <v>6.5888812628689102E-3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -7905,16 +7916,16 @@
       <c r="B26" s="1"/>
       <c r="C26">
         <f>LHeartSmallVesselGradient</f>
-        <v>91.5</v>
+        <v>89.5</v>
       </c>
       <c r="D26" s="6">
         <f>LHeartFlowMale/LHeartSmallVesselGradient</f>
-        <v>1.9593442622950821</v>
+        <v>2.0031284916201115</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="4">
         <f>D26/E24</f>
-        <v>6.6968957098011879E-3</v>
+        <v>6.8465470105788673E-3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -7927,11 +7938,11 @@
       </c>
       <c r="C27">
         <f>CoronaryGradient</f>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D27" s="6">
         <f>B27/C27</f>
-        <v>0.38652631578947377</v>
+        <v>0.39483870967741941</v>
       </c>
       <c r="E27" s="1">
         <f>RHeartMassMale</f>
@@ -7939,7 +7950,7 @@
       </c>
       <c r="F27" s="4">
         <f>D27/E27</f>
-        <v>6.4501679731243022E-3</v>
+        <v>6.5888812628689102E-3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -7968,21 +7979,21 @@
       <c r="B29" s="1"/>
       <c r="C29">
         <f>RHeartSmallVesselGradient</f>
-        <v>91.5</v>
+        <v>89.5</v>
       </c>
       <c r="D29" s="6">
         <f>RHeartFlowMale/RHeartSmallVesselGradient</f>
-        <v>0.40131147540983614</v>
+        <v>0.41027932960893859</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="4">
         <f>D29/E27</f>
-        <v>6.696895709801187E-3</v>
+        <v>6.8465470105788673E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B30" s="1">
         <f>SUM(B24:B27)</f>
@@ -7996,7 +8007,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1">
         <f>SystemicVeinOutflow+HepaticVeinOutflow+CoronarySinusOutflow</f>
@@ -8009,7 +8020,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B34">
         <f>VenousReturn</f>
@@ -8027,7 +8038,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35">
         <f>VenousReturn</f>
@@ -8035,17 +8046,17 @@
       </c>
       <c r="C35">
         <f>PulmCapysGradient</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
         <f>B35/C35</f>
-        <v>1800</v>
+        <v>5400</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B36">
         <f>VenousReturn</f>
@@ -8082,7 +8093,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8095,27 +8106,27 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B5" s="1">
         <f>BaseMassMale</f>
@@ -8223,7 +8234,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1">
         <f>OrganMassMale</f>

</xml_diff>

<commit_message>
2013-02-18. Current log. HumMod version bumped to 2.0.51. Adding mass balance for 20 amino acids -- 10 essential and 10 non-essential. First compartments are extracellular, in Structure\AminoAcid. Structure names have AA- prefix. Panel is at Metabolism | Amino Acids | ECFV.
Under development but not completed is scaling the vascular compartments at startup so that the model is context sensitive but not parameter sensitive. Coming next.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
     <sheet name="Organ Mass - Male" sheetId="4" r:id="rId2"/>
     <sheet name="Organ Mass - Female" sheetId="5" r:id="rId3"/>
     <sheet name="Blood Pressures" sheetId="6" r:id="rId4"/>
-    <sheet name="Pressure Gradients" sheetId="9" r:id="rId5"/>
-    <sheet name="Organ Composition" sheetId="1" r:id="rId6"/>
-    <sheet name="Organ Blood Flow" sheetId="7" r:id="rId7"/>
-    <sheet name="Flows &amp; Conductances" sheetId="10" r:id="rId8"/>
-    <sheet name="Cardiac Output" sheetId="13" r:id="rId9"/>
-    <sheet name="Blood Volume" sheetId="12" r:id="rId10"/>
-    <sheet name="Calories Used" sheetId="2" r:id="rId11"/>
-    <sheet name="Insulin Receptors" sheetId="14" r:id="rId12"/>
-    <sheet name="PV-Arteries" sheetId="15" r:id="rId13"/>
-    <sheet name="PV-Veins" sheetId="16" r:id="rId14"/>
-    <sheet name="PV-Lungs" sheetId="17" r:id="rId15"/>
+    <sheet name="Compartments" sheetId="18" r:id="rId5"/>
+    <sheet name="Pressure Gradients" sheetId="9" r:id="rId6"/>
+    <sheet name="Organ Composition" sheetId="1" r:id="rId7"/>
+    <sheet name="Organ Blood Flow" sheetId="7" r:id="rId8"/>
+    <sheet name="Flows &amp; Conductances" sheetId="10" r:id="rId9"/>
+    <sheet name="Cardiac Output" sheetId="13" r:id="rId10"/>
+    <sheet name="Blood Volume" sheetId="12" r:id="rId11"/>
+    <sheet name="Calories Used" sheetId="2" r:id="rId12"/>
+    <sheet name="Insulin Receptors" sheetId="14" r:id="rId13"/>
+    <sheet name="PV-Arteries" sheetId="15" r:id="rId14"/>
+    <sheet name="PV-Veins" sheetId="16" r:id="rId15"/>
+    <sheet name="PV-Lungs" sheetId="17" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
@@ -56,6 +57,9 @@
     <definedName name="CoronarySinusOutflow">'Flows &amp; Conductances'!$B$30</definedName>
     <definedName name="Density">'PV-Arteries'!$G$3</definedName>
     <definedName name="EfferentArtyGradient">'Pressure Gradients'!$D$9</definedName>
+    <definedName name="F_BV_Arteries">'PV-Arteries'!$B$3</definedName>
+    <definedName name="F_BV_Lungs">'PV-Arteries'!$D$3</definedName>
+    <definedName name="F_BV_Veins">'PV-Arteries'!$C$3</definedName>
     <definedName name="FatFlowFemale">'Organ Blood Flow'!$H$9</definedName>
     <definedName name="FatFlowGFemale">'Organ Blood Flow'!$J$9</definedName>
     <definedName name="FatFlowGMale">'Organ Blood Flow'!$E$9</definedName>
@@ -154,6 +158,14 @@
     <definedName name="SystemicVeinsPressure">'Blood Pressures'!$B$12</definedName>
     <definedName name="ThyroidMassFemale">'Organ Mass - Female'!$D$36</definedName>
     <definedName name="ThyroidMassMale">'Organ Mass - Male'!$C$42</definedName>
+    <definedName name="TMP_LeftAtrium">'Blood Pressures'!$D$18</definedName>
+    <definedName name="TMP_PulmonaryArtery">'Blood Pressures'!$D$15</definedName>
+    <definedName name="TMP_PulmonaryCapillaries">'Blood Pressures'!$D$16</definedName>
+    <definedName name="TMP_PulmonaryVeins">'Blood Pressures'!$D$17</definedName>
+    <definedName name="TMP_RightAtrium">'Blood Pressures'!$D$14</definedName>
+    <definedName name="TMP_SplanchnicVeins">'Blood Pressures'!$D$13</definedName>
+    <definedName name="TMP_SystemicArteries">'Blood Pressures'!$D$4</definedName>
+    <definedName name="TMP_SystemicVeins">'Blood Pressures'!$D$12</definedName>
     <definedName name="VenousReturn">'Flows &amp; Conductances'!$B$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -197,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="230">
   <si>
     <t>Bone</t>
   </si>
@@ -848,6 +860,45 @@
   </si>
   <si>
     <t>Splanchnic Vein</t>
+  </si>
+  <si>
+    <t>Compartments</t>
+  </si>
+  <si>
+    <t>Veins</t>
+  </si>
+  <si>
+    <t>Sequestered</t>
+  </si>
+  <si>
+    <t>Artery</t>
+  </si>
+  <si>
+    <t>Capillaries</t>
+  </si>
+  <si>
+    <t>Peripheral</t>
+  </si>
+  <si>
+    <t>Caronary Sinus</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>Blood Flow ====</t>
+  </si>
+  <si>
+    <t>Veins ========</t>
+  </si>
+  <si>
+    <t>Lungs ========</t>
+  </si>
+  <si>
+    <t>Arteries ======</t>
+  </si>
+  <si>
+    <t>V0-F</t>
   </si>
 </sst>
 </file>
@@ -1298,6 +1349,187 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="1">
+        <f>BaseMassMale</f>
+        <v>26032.5</v>
+      </c>
+      <c r="C5" s="7">
+        <f>BaseFlowGMale</f>
+        <v>0.16602938634399309</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5*B5</f>
+        <v>4322.16</v>
+      </c>
+      <c r="F5" s="1">
+        <f>BaseMassFemale</f>
+        <v>20794.799999999996</v>
+      </c>
+      <c r="G5" s="7">
+        <f>BaseFlowGFemale</f>
+        <v>0.17052149722811896</v>
+      </c>
+      <c r="H5" s="1">
+        <f>G5*F5</f>
+        <v>3545.9604305592875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+      <c r="C6" s="7">
+        <f>SMuscleFlowGMale</f>
+        <v>3.0600000000000006E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <f>C6*B6</f>
+        <v>807.84000000000015</v>
+      </c>
+      <c r="F6" s="1">
+        <f>SMuscleMassFemale</f>
+        <v>14628.900000000001</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SMuscleFlowGFemale</f>
+        <v>2.983721055176489E-2</v>
+      </c>
+      <c r="H6" s="1">
+        <f>G6*F6</f>
+        <v>436.48556944071345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
+      </c>
+      <c r="C7" s="7">
+        <f>FatFlowGMale</f>
+        <v>1.6822429906542057E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7*B7</f>
+        <v>270</v>
+      </c>
+      <c r="F7" s="1">
+        <f>FatMassFemale</f>
+        <v>19767.150000000001</v>
+      </c>
+      <c r="G7" s="7">
+        <f>FatFlowGFemale</f>
+        <v>1.8715596330275232E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <f>G7*F7</f>
+        <v>369.95400000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <f>SUM(B5:B7)</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D8" s="1">
+        <f>SUM(D5:D7)</f>
+        <v>5400</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUM(F5:F7)</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUM(H5:H7)</f>
+        <v>4352.4000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="1">
+        <f>OrganMassMale</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D9" s="1">
+        <f>CardiacOutputMale</f>
+        <v>5400</v>
+      </c>
+      <c r="F9" s="1">
+        <f>OrganMassFemale</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H9" s="1">
+        <f>CardiacOutputFemale</f>
+        <v>4352.4000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1517,7 +1749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -1882,7 +2114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -2165,12 +2397,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,11 +3331,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -4115,11 +4347,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5303,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,10 +5890,383 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1">
+        <f>BloodVolume_Male</f>
+        <v>5407.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="1">
+        <f>BloodVolume_Male_Arteries</f>
+        <v>973.43099999999993</v>
+      </c>
+      <c r="C6">
+        <f>F_BV_Arteries</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="1">
+        <f>C7*B6</f>
+        <v>924.7594499999999</v>
+      </c>
+      <c r="C7">
+        <f>1-C8</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="1">
+        <f>C8*B6</f>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" s="1">
+        <f>SUM(B7:B8)</f>
+        <v>973.43099999999993</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C7:C8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="1">
+        <f>BloodVolume_Male_Veins</f>
+        <v>3623.3265000000001</v>
+      </c>
+      <c r="C11">
+        <f>F_BV_Veins</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="1">
+        <f>C12*B11</f>
+        <v>2311.682307</v>
+      </c>
+      <c r="C12">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="1">
+        <f>C13*B11</f>
+        <v>1014.5314200000001</v>
+      </c>
+      <c r="C13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1">
+        <f>C14*B11</f>
+        <v>50.726571</v>
+      </c>
+      <c r="C14">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="1">
+        <f>C15*B11</f>
+        <v>94.206489000000005</v>
+      </c>
+      <c r="C15">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="1">
+        <f>C16*B11</f>
+        <v>152.17971300000002</v>
+      </c>
+      <c r="C16">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17" s="1">
+        <f>SUM(B12:B16)</f>
+        <v>3623.3265000000006</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C12:C16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" s="1">
+        <f>BloodVolume_Male_Lungs</f>
+        <v>811.1925</v>
+      </c>
+      <c r="C19">
+        <f>F_BV_Lungs</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="1">
+        <f>B19*C20</f>
+        <v>219.02197500000003</v>
+      </c>
+      <c r="C20">
+        <v>0.27</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f>D20*B20</f>
+        <v>109.51098750000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="1">
+        <f>B19*C21</f>
+        <v>219.02197500000003</v>
+      </c>
+      <c r="C21">
+        <v>0.27</v>
+      </c>
+      <c r="D21">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="1">
+        <f>D21*B21</f>
+        <v>131.413185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" s="1">
+        <f>B19*C22</f>
+        <v>235.245825</v>
+      </c>
+      <c r="C22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.6</v>
+      </c>
+      <c r="E22" s="1">
+        <f>D22*B22</f>
+        <v>141.14749499999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1">
+        <f>B19*C23</f>
+        <v>48.671549999999996</v>
+      </c>
+      <c r="C23">
+        <v>0.06</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f>D23*B23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="1">
+        <f>B19*C24</f>
+        <v>89.231174999999993</v>
+      </c>
+      <c r="C24">
+        <v>0.11</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <f>D24*B24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" s="1">
+        <f>SUM(B20:B24)</f>
+        <v>811.19250000000011</v>
+      </c>
+      <c r="C25">
+        <f>SUM(C20:C24)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <f>CardiacOutputMale</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31">
+        <f>SystemicVeinOutflow</f>
+        <v>3834</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32">
+        <f>HepaticVeinOutflow</f>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33">
+        <f>CoronarySinusOutflow</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>224</v>
+      </c>
+      <c r="B34">
+        <f>SUM(B31:B33)</f>
+        <v>5400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,7 +6567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -6490,7 +7097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
@@ -7442,12 +8049,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8076,185 +8683,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="1">
-        <f>BaseMassMale</f>
-        <v>26032.5</v>
-      </c>
-      <c r="C5" s="7">
-        <f>BaseFlowGMale</f>
-        <v>0.16602938634399309</v>
-      </c>
-      <c r="D5" s="1">
-        <f>C5*B5</f>
-        <v>4322.16</v>
-      </c>
-      <c r="F5" s="1">
-        <f>BaseMassFemale</f>
-        <v>20794.799999999996</v>
-      </c>
-      <c r="G5" s="7">
-        <f>BaseFlowGFemale</f>
-        <v>0.17052149722811896</v>
-      </c>
-      <c r="H5" s="1">
-        <f>G5*F5</f>
-        <v>3545.9604305592875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="1">
-        <f>SMuscleMassMale</f>
-        <v>26400</v>
-      </c>
-      <c r="C6" s="7">
-        <f>SMuscleFlowGMale</f>
-        <v>3.0600000000000006E-2</v>
-      </c>
-      <c r="D6" s="1">
-        <f>C6*B6</f>
-        <v>807.84000000000015</v>
-      </c>
-      <c r="F6" s="1">
-        <f>SMuscleMassFemale</f>
-        <v>14628.900000000001</v>
-      </c>
-      <c r="G6" s="7">
-        <f>SMuscleFlowGFemale</f>
-        <v>2.983721055176489E-2</v>
-      </c>
-      <c r="H6" s="1">
-        <f>G6*F6</f>
-        <v>436.48556944071345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <f>FatMassMale</f>
-        <v>16050</v>
-      </c>
-      <c r="C7" s="7">
-        <f>FatFlowGMale</f>
-        <v>1.6822429906542057E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <f>C7*B7</f>
-        <v>270</v>
-      </c>
-      <c r="F7" s="1">
-        <f>FatMassFemale</f>
-        <v>19767.150000000001</v>
-      </c>
-      <c r="G7" s="7">
-        <f>FatFlowGFemale</f>
-        <v>1.8715596330275232E-2</v>
-      </c>
-      <c r="H7" s="1">
-        <f>G7*F7</f>
-        <v>369.95400000000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1">
-        <f>SUM(B5:B7)</f>
-        <v>68482.5</v>
-      </c>
-      <c r="D8" s="1">
-        <f>SUM(D5:D7)</f>
-        <v>5400</v>
-      </c>
-      <c r="F8" s="1">
-        <f>SUM(F5:F7)</f>
-        <v>55190.85</v>
-      </c>
-      <c r="H8" s="1">
-        <f>SUM(H5:H7)</f>
-        <v>4352.4000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="1">
-        <f>OrganMassMale</f>
-        <v>68482.5</v>
-      </c>
-      <c r="D9" s="1">
-        <f>CardiacOutputMale</f>
-        <v>5400</v>
-      </c>
-      <c r="F9" s="1">
-        <f>OrganMassFemale</f>
-        <v>55190.85</v>
-      </c>
-      <c r="H9" s="1">
-        <f>CardiacOutputFemale</f>
-        <v>4352.4000000000005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
2013-02-22 HumMod v2.0.52. Pushing current log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -178,6 +178,42 @@
     <author>Tom Coleman</author>
   </authors>
   <commentList>
+    <comment ref="G3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom Coleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+P = (1/C) * (V - V0)
+rearranging and using TMP
+C = (1/TMP) * (V - V0)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tom Coleman</author>
+  </authors>
+  <commentList>
     <comment ref="B5" authorId="0">
       <text>
         <r>
@@ -209,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="233">
   <si>
     <t>Bone</t>
   </si>
@@ -899,6 +935,15 @@
   </si>
   <si>
     <t>V0-F</t>
+  </si>
+  <si>
+    <t>Circulating</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Rounded</t>
   </si>
 </sst>
 </file>
@@ -911,7 +956,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -938,6 +983,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1349,15 +1407,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1518,6 +1577,135 @@
         <v>55190.85</v>
       </c>
       <c r="H9" s="1">
+        <f>CardiacOutputFemale</f>
+        <v>4352.4000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="1">
+        <v>26000</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.16619999999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <f>C12*B12</f>
+        <v>4321.2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>BaseMassFemale</f>
+        <v>20794.799999999996</v>
+      </c>
+      <c r="G12" s="7">
+        <f>BaseFlowGFemale</f>
+        <v>0.17052149722811896</v>
+      </c>
+      <c r="H12" s="1">
+        <f>G12*F12</f>
+        <v>3545.9604305592875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <f>C13*B13</f>
+        <v>807.83999999999992</v>
+      </c>
+      <c r="F13" s="1">
+        <f>SMuscleMassFemale</f>
+        <v>14628.900000000001</v>
+      </c>
+      <c r="G13" s="7">
+        <f>SMuscleFlowGFemale</f>
+        <v>2.983721055176489E-2</v>
+      </c>
+      <c r="H13" s="1">
+        <f>G13*F13</f>
+        <v>436.48556944071345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>16100</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <f>C14*B14</f>
+        <v>270.47999999999996</v>
+      </c>
+      <c r="F14" s="1">
+        <f>FatMassFemale</f>
+        <v>19767.150000000001</v>
+      </c>
+      <c r="G14" s="7">
+        <f>FatFlowGFemale</f>
+        <v>1.8715596330275232E-2</v>
+      </c>
+      <c r="H14" s="1">
+        <f>G14*F14</f>
+        <v>369.95400000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1">
+        <f>SUM(B12:B14)</f>
+        <v>68500</v>
+      </c>
+      <c r="D15" s="1">
+        <f>SUM(D12:D14)</f>
+        <v>5399.5199999999995</v>
+      </c>
+      <c r="F15" s="1">
+        <f>SUM(F12:F14)</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(H12:H14)</f>
+        <v>4352.4000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="1">
+        <f>OrganMassMale</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D16" s="1">
+        <f>CardiacOutputMale</f>
+        <v>5400</v>
+      </c>
+      <c r="F16" s="1">
+        <f>OrganMassFemale</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H16" s="1">
         <f>CardiacOutputFemale</f>
         <v>4352.4000000000005</v>
       </c>
@@ -5889,11 +6077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5901,12 +6089,12 @@
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -5923,8 +6111,11 @@
       <c r="F3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -5933,7 +6124,7 @@
         <v>5407.95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>228</v>
       </c>
@@ -5946,318 +6137,406 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B6-B7</f>
+        <v>923.43099999999993</v>
+      </c>
+      <c r="D8">
+        <v>0.85</v>
+      </c>
+      <c r="E8" s="1">
+        <f>D8*B8</f>
+        <v>784.91634999999997</v>
+      </c>
+      <c r="F8">
+        <f>TMP_SystemicArteries</f>
+        <v>97</v>
+      </c>
+      <c r="G8" s="6">
+        <f>(1/F8)*(B8-E8)</f>
+        <v>1.4279860824742263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="1">
-        <f>C7*B6</f>
-        <v>924.7594499999999</v>
-      </c>
-      <c r="C7">
-        <f>1-C8</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B8" s="1">
-        <f>C8*B6</f>
-        <v>48.671549999999996</v>
-      </c>
-      <c r="C8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="1">
+        <f>C9*B8</f>
+        <v>923.43099999999993</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>224</v>
       </c>
-      <c r="B9" s="1">
-        <f>SUM(B7:B8)</f>
-        <v>973.43099999999993</v>
-      </c>
-      <c r="C9">
-        <f>SUM(C7:C8)</f>
+      <c r="B10" s="1">
+        <f>SUM(B9:B9)</f>
+        <v>923.43099999999993</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C9:C9)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>226</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <f>BloodVolume_Male_Veins</f>
         <v>3623.3265000000001</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f>F_BV_Veins</f>
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="1">
-        <f>C12*B11</f>
-        <v>2311.682307</v>
-      </c>
-      <c r="C12">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="D12">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="1">
+        <f>B12-B13-B14</f>
+        <v>3373.3265000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" s="1">
+        <f>C16*B15</f>
+        <v>2310.7286525</v>
+      </c>
+      <c r="C16">
+        <f>1-C17-C18</f>
+        <v>0.68499999999999994</v>
+      </c>
+      <c r="D16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E16" s="1">
+        <f>D16*B16</f>
+        <v>1155.36432625</v>
+      </c>
+      <c r="F16">
+        <f>TMP_SystemicVeins</f>
+        <v>10</v>
+      </c>
+      <c r="G16" s="5">
+        <f>(1/F16)*(B16-E16)</f>
+        <v>115.536432625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>185</v>
       </c>
-      <c r="B13" s="1">
-        <f>C13*B11</f>
-        <v>1014.5314200000001</v>
-      </c>
-      <c r="C13">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D13">
+      <c r="B17" s="1">
+        <f>C17*B15</f>
+        <v>1011.9979499999999</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+      <c r="D17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E17" s="1">
+        <f>D17*B17</f>
+        <v>505.99897499999997</v>
+      </c>
+      <c r="F17">
+        <f>TMP_SplanchnicVeins</f>
+        <v>8</v>
+      </c>
+      <c r="G17" s="5">
+        <f>(1/F17)*(B17-E17)</f>
+        <v>63.249871874999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="1">
-        <f>C14*B11</f>
-        <v>50.726571</v>
-      </c>
-      <c r="C14">
-        <v>1.4E-2</v>
-      </c>
-      <c r="D14">
+      <c r="B18" s="1">
+        <f>C18*B15</f>
+        <v>50.599897499999997</v>
+      </c>
+      <c r="C18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B15" s="1">
-        <f>C15*B11</f>
-        <v>94.206489000000005</v>
-      </c>
-      <c r="C15">
-        <v>2.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>219</v>
-      </c>
-      <c r="B16" s="1">
-        <f>C16*B11</f>
-        <v>152.17971300000002</v>
-      </c>
-      <c r="C16">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E18" s="1">
+        <f>D18*B18</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>TMP_RightAtrium</f>
+        <v>7</v>
+      </c>
+      <c r="G18" s="6">
+        <f>(1/F18)*(B18-E18)</f>
+        <v>7.2285567857142849</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>224</v>
       </c>
-      <c r="B17" s="1">
-        <f>SUM(B12:B16)</f>
-        <v>3623.3265000000006</v>
-      </c>
-      <c r="C17">
-        <f>SUM(C12:C16)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" s="1">
+        <f>SUM(B16:B18)</f>
+        <v>3373.3265000000001</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C16:C18)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>227</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B21" s="1">
         <f>BloodVolume_Male_Lungs</f>
         <v>811.1925</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <f>F_BV_Lungs</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" s="1">
+        <f>B21-B22</f>
+        <v>711.1925</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="1">
-        <f>B19*C20</f>
-        <v>219.02197500000003</v>
-      </c>
-      <c r="C20">
-        <v>0.27</v>
-      </c>
-      <c r="D20">
+      <c r="B24" s="1">
+        <f>B23*C24</f>
+        <v>220.469675</v>
+      </c>
+      <c r="C24">
+        <v>0.31</v>
+      </c>
+      <c r="D24">
         <v>0.5</v>
-      </c>
-      <c r="E20" s="1">
-        <f>D20*B20</f>
-        <v>109.51098750000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>221</v>
-      </c>
-      <c r="B21" s="1">
-        <f>B19*C21</f>
-        <v>219.02197500000003</v>
-      </c>
-      <c r="C21">
-        <v>0.27</v>
-      </c>
-      <c r="D21">
-        <v>0.6</v>
-      </c>
-      <c r="E21" s="1">
-        <f>D21*B21</f>
-        <v>131.413185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" s="1">
-        <f>B19*C22</f>
-        <v>235.245825</v>
-      </c>
-      <c r="C22">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D22">
-        <v>0.6</v>
-      </c>
-      <c r="E22" s="1">
-        <f>D22*B22</f>
-        <v>141.14749499999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="1">
-        <f>B19*C23</f>
-        <v>48.671549999999996</v>
-      </c>
-      <c r="C23">
-        <v>0.06</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <f>D23*B23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>190</v>
-      </c>
-      <c r="B24" s="1">
-        <f>B19*C24</f>
-        <v>89.231174999999993</v>
-      </c>
-      <c r="C24">
-        <v>0.11</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
       </c>
       <c r="E24" s="1">
         <f>D24*B24</f>
+        <v>110.2348375</v>
+      </c>
+      <c r="F24">
+        <f>TMP_PulmonaryArtery</f>
+        <v>18</v>
+      </c>
+      <c r="G24" s="6">
+        <f>(1/F24)*(B24-E24)</f>
+        <v>6.1241576388888888</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>221</v>
+      </c>
+      <c r="B25" s="1">
+        <f>B23*C25</f>
+        <v>213.35774999999998</v>
+      </c>
+      <c r="C25">
+        <v>0.3</v>
+      </c>
+      <c r="D25">
+        <v>0.6</v>
+      </c>
+      <c r="E25" s="1">
+        <f>D25*B25</f>
+        <v>128.01464999999999</v>
+      </c>
+      <c r="F25">
+        <f>TMP_PulmonaryCapillaries</f>
+        <v>14</v>
+      </c>
+      <c r="G25" s="6">
+        <f>(1/F25)*(B25-E25)</f>
+        <v>6.0959357142857131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" s="1">
+        <f>B23*C26</f>
+        <v>227.58160000000001</v>
+      </c>
+      <c r="C26">
+        <v>0.32</v>
+      </c>
+      <c r="D26">
+        <v>0.6</v>
+      </c>
+      <c r="E26" s="1">
+        <f>D26*B26</f>
+        <v>136.54895999999999</v>
+      </c>
+      <c r="F26">
+        <f>TMP_PulmonaryVeins</f>
+        <v>13</v>
+      </c>
+      <c r="G26" s="6">
+        <f>(1/F26)*(B26-E26)</f>
+        <v>7.0025107692307706</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1">
+        <f>B23*C27</f>
+        <v>49.783475000000003</v>
+      </c>
+      <c r="C27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="E27" s="1">
+        <f>D27*B27</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>TMP_LeftAtrium</f>
+        <v>11</v>
+      </c>
+      <c r="G27" s="6">
+        <f>(1/F27)*(B27-E27)</f>
+        <v>4.5257704545454551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>224</v>
       </c>
-      <c r="B25" s="1">
-        <f>SUM(B20:B24)</f>
-        <v>811.19250000000011</v>
-      </c>
-      <c r="C25">
-        <f>SUM(C20:C24)</f>
-        <v>1.0000000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B28" s="1">
+        <f>SUM(B24:B27)</f>
+        <v>711.19249999999988</v>
+      </c>
+      <c r="C28">
+        <f>SUM(C24:C27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B30">
+      <c r="B33">
         <f>CardiacOutputMale</f>
         <v>5400</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>222</v>
       </c>
-      <c r="B31">
+      <c r="B34">
         <f>SystemicVeinOutflow</f>
         <v>3834</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>185</v>
       </c>
-      <c r="B32">
+      <c r="B35">
         <f>HepaticVeinOutflow</f>
         <v>1350</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>223</v>
       </c>
-      <c r="B33">
+      <c r="B36">
         <f>CoronarySinusOutflow</f>
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>224</v>
       </c>
-      <c r="B34">
-        <f>SUM(B31:B33)</f>
+      <c r="B37">
+        <f>SUM(B34:B36)</f>
         <v>5400</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7101,8 +7380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8053,8 +8332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2013-02-26 HumMod v2.0.54. Current log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <sheet name="Organ Blood Flow" sheetId="7" r:id="rId8"/>
     <sheet name="Flows &amp; Conductances" sheetId="10" r:id="rId9"/>
     <sheet name="Cardiac Output" sheetId="13" r:id="rId10"/>
-    <sheet name="Blood Volume" sheetId="12" r:id="rId11"/>
-    <sheet name="Calories Used" sheetId="2" r:id="rId12"/>
-    <sheet name="Insulin Receptors" sheetId="14" r:id="rId13"/>
-    <sheet name="PV-Arteries" sheetId="15" r:id="rId14"/>
-    <sheet name="PV-Veins" sheetId="16" r:id="rId15"/>
-    <sheet name="PV-Lungs" sheetId="17" r:id="rId16"/>
+    <sheet name="Osmoles" sheetId="19" r:id="rId11"/>
+    <sheet name="Blood Volume" sheetId="12" r:id="rId12"/>
+    <sheet name="Calories Used" sheetId="2" r:id="rId13"/>
+    <sheet name="Insulin Receptors" sheetId="14" r:id="rId14"/>
+    <sheet name="PV-Arteries" sheetId="15" r:id="rId15"/>
+    <sheet name="PV-Veins" sheetId="16" r:id="rId16"/>
+    <sheet name="PV-Lungs" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
@@ -53,10 +54,13 @@
     <definedName name="BrainMassMale">'Organ Mass - Male'!$C$5</definedName>
     <definedName name="CardiacOutputFemale">'Organ Blood Flow'!$D$5</definedName>
     <definedName name="CardiacOutputMale">'Organ Blood Flow'!$D$4</definedName>
+    <definedName name="Cell_H2O">'Organ Composition'!$D$31</definedName>
     <definedName name="CoronaryGradient">'Pressure Gradients'!$D$6</definedName>
     <definedName name="CoronarySinusOutflow">'Flows &amp; Conductances'!$B$30</definedName>
     <definedName name="Density">'PV-Arteries'!$G$3</definedName>
+    <definedName name="ECFV_H2O">'Organ Composition'!$D$32</definedName>
     <definedName name="EfferentArtyGradient">'Pressure Gradients'!$D$9</definedName>
+    <definedName name="External_H2O">'Organ Composition'!$D$33</definedName>
     <definedName name="F_BV_Arteries">'PV-Arteries'!$B$3</definedName>
     <definedName name="F_BV_Lungs">'PV-Arteries'!$D$3</definedName>
     <definedName name="F_BV_Veins">'PV-Arteries'!$C$3</definedName>
@@ -166,6 +170,7 @@
     <definedName name="TMP_SplanchnicVeins">'Blood Pressures'!$D$13</definedName>
     <definedName name="TMP_SystemicArteries">'Blood Pressures'!$D$4</definedName>
     <definedName name="TMP_SystemicVeins">'Blood Pressures'!$D$12</definedName>
+    <definedName name="Total_H2O">'Organ Composition'!$D$34</definedName>
     <definedName name="VenousReturn">'Flows &amp; Conductances'!$B$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -245,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="264">
   <si>
     <t>Bone</t>
   </si>
@@ -944,6 +949,99 @@
   </si>
   <si>
     <t>Rounded</t>
+  </si>
+  <si>
+    <t>Osmoles</t>
+  </si>
+  <si>
+    <t>ECFV</t>
+  </si>
+  <si>
+    <t>Dissociation</t>
+  </si>
+  <si>
+    <t>H20 Mass</t>
+  </si>
+  <si>
+    <t>H2O Total</t>
+  </si>
+  <si>
+    <t>ECFV-F</t>
+  </si>
+  <si>
+    <t>Cell-F</t>
+  </si>
+  <si>
+    <t>Gut</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>[Osm]</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Receptor</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Na+</t>
+  </si>
+  <si>
+    <t>K+</t>
+  </si>
+  <si>
+    <t>Total Anions</t>
+  </si>
+  <si>
+    <t>Total Cations</t>
+  </si>
+  <si>
+    <t>Total Ions</t>
+  </si>
+  <si>
+    <t>ECFV =========</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>Urea</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Total Osmoles</t>
+  </si>
+  <si>
+    <t>Cell ==========</t>
+  </si>
+  <si>
+    <t>Check Math []</t>
+  </si>
+  <si>
+    <t>Total ! Ions</t>
+  </si>
+  <si>
+    <t>Active Ions</t>
+  </si>
+  <si>
+    <t>Total Active</t>
+  </si>
+  <si>
+    <t>Check Maht []</t>
   </si>
 </sst>
 </file>
@@ -1718,6 +1816,446 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2">
+        <v>0.93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>302</v>
+      </c>
+      <c r="C3">
+        <v>282</v>
+      </c>
+      <c r="F3">
+        <f>Total_H2O</f>
+        <v>43019.367120000003</v>
+      </c>
+      <c r="G3">
+        <f>Cell_H2O</f>
+        <v>27010.059615000002</v>
+      </c>
+      <c r="H3">
+        <f>ECFV_H2O</f>
+        <v>15034.307505000001</v>
+      </c>
+      <c r="I3">
+        <f>External_H2O</f>
+        <v>975</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="5">
+        <f>F3/1000</f>
+        <v>43.019367120000005</v>
+      </c>
+      <c r="G4" s="5">
+        <f>G3/1000</f>
+        <v>27.010059615000003</v>
+      </c>
+      <c r="H4" s="5">
+        <f>H3/1000</f>
+        <v>15.034307505000001</v>
+      </c>
+      <c r="I4" s="5">
+        <f>I3/1000</f>
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7">
+        <v>144</v>
+      </c>
+      <c r="C7" s="1">
+        <f>B7*H4</f>
+        <v>2164.9402807200004</v>
+      </c>
+      <c r="E7" s="1">
+        <f>C7</f>
+        <v>2164.9402807200004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C8" s="1">
+        <f>B8*H4</f>
+        <v>66.15095302200001</v>
+      </c>
+      <c r="E8" s="1">
+        <f>C8</f>
+        <v>66.15095302200001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C7:C8)</f>
+        <v>2231.0912337420004</v>
+      </c>
+      <c r="E9" s="1">
+        <f>C9</f>
+        <v>2231.0912337420004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="1">
+        <f>C9</f>
+        <v>2231.0912337420004</v>
+      </c>
+      <c r="E10" s="1">
+        <f>C10</f>
+        <v>2231.0912337420004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" s="1">
+        <f>C9+C10</f>
+        <v>4462.1824674840009</v>
+      </c>
+      <c r="E11" s="1">
+        <f>C11</f>
+        <v>4462.1824674840009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" s="1">
+        <f>E2*C11</f>
+        <v>4149.8296947601211</v>
+      </c>
+      <c r="E12" s="1">
+        <f>C12</f>
+        <v>4149.8296947601211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14">
+        <v>5.5</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B14*H4</f>
+        <v>82.688691277499998</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <f>B15*H4</f>
+        <v>60.137230020000004</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f>C16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="1">
+        <f>SUM(C14:C16)</f>
+        <v>142.8259212975</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUM(C11,C17)</f>
+        <v>4605.0083887815008</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUM(E11,E17)</f>
+        <v>4462.1824674840009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" s="1">
+        <f>C19/H4</f>
+        <v>306.3</v>
+      </c>
+      <c r="E20" s="1">
+        <f>E19/H4</f>
+        <v>296.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" s="1">
+        <f>SUM(C12,C17)</f>
+        <v>4292.655616057621</v>
+      </c>
+      <c r="E22" s="1">
+        <f>SUM(E12,E17)</f>
+        <v>4149.8296947601211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23" s="1">
+        <f>C22/H4</f>
+        <v>285.52400000000006</v>
+      </c>
+      <c r="E23" s="1">
+        <f>E22/H4</f>
+        <v>276.02400000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>249</v>
+      </c>
+      <c r="B27">
+        <v>140</v>
+      </c>
+      <c r="C27" s="1">
+        <f>B27*G4</f>
+        <v>3781.4083461000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1">
+        <f>B28*G4</f>
+        <v>270.10059615</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="1">
+        <f>SUM(C27:C28)</f>
+        <v>4051.5089422500005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C30" s="1">
+        <f>C29</f>
+        <v>4051.5089422500005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C31" s="1">
+        <f>C29+C30</f>
+        <v>8103.0178845000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C32" s="1">
+        <f>E2*C31</f>
+        <v>7535.8066325850014</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>255</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1">
+        <f>B34*G4</f>
+        <v>108.04023846000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>256</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
+        <f>B35*G4</f>
+        <v>54.020119230000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>260</v>
+      </c>
+      <c r="C36" s="1">
+        <f>C34+C35</f>
+        <v>162.06035769000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>257</v>
+      </c>
+      <c r="C38" s="1">
+        <f>C31+C36</f>
+        <v>8265.0782421900003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>263</v>
+      </c>
+      <c r="C39">
+        <f>C38/G4</f>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>262</v>
+      </c>
+      <c r="C41" s="1">
+        <f>C32+C36</f>
+        <v>7697.8669902750016</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>259</v>
+      </c>
+      <c r="C42">
+        <f>C41/G4</f>
+        <v>285.00000000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1937,7 +2475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -2302,7 +2840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -2585,7 +3123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
@@ -3519,7 +4057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -4535,7 +5073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -6080,7 +6618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -6848,16 +7386,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B16"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
@@ -7269,7 +7807,7 @@
         <v>31098.974999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -7278,7 +7816,7 @@
         <v>5550</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -7286,7 +7824,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -7294,8 +7832,12 @@
         <f>B18*(1-Hematocrit)</f>
         <v>3108.0000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>B20</f>
+        <v>3108.0000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -7307,7 +7849,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -7315,8 +7857,12 @@
         <f>B21*C21</f>
         <v>1611.72</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <f>B22</f>
+        <v>1611.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -7325,7 +7871,7 @@
         <v>830.28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -7333,8 +7879,12 @@
         <f>LungH2OMass</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>B24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -7342,8 +7892,12 @@
         <f>PeritoneumMass</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>B25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -7351,8 +7905,12 @@
         <f>GutH2OMass</f>
         <v>975</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f>B26</f>
+        <v>975</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -7360,14 +7918,67 @@
         <f>FluidsMass</f>
         <v>6525</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="1">
+        <f>SUM(D20,D22,D24,D25,D26)</f>
+        <v>5694.72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="1">
         <f>B16+B27</f>
         <v>75007.5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>237</v>
+      </c>
+      <c r="D29" s="1">
+        <f>SUM(D16,D27)</f>
+        <v>43078.245000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>239</v>
+      </c>
+      <c r="C31">
+        <v>0.627</v>
+      </c>
+      <c r="D31">
+        <f>C31*D29</f>
+        <v>27010.059615000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32">
+        <f xml:space="preserve"> 0.349</f>
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="D32">
+        <f>C32*D29</f>
+        <v>15034.307505000001</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>240</v>
+      </c>
+      <c r="D33">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f>SUM(D31:D33)</f>
+        <v>43019.367120000003</v>
       </c>
     </row>
   </sheetData>
@@ -8333,7 +8944,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8743,8 +9354,14 @@
         <f>B22/C22</f>
         <v>337.5</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="1">
+        <f>E20</f>
+        <v>1950</v>
+      </c>
+      <c r="F22" s="4">
+        <f>D22/E22</f>
+        <v>0.17307692307692307</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>

</xml_diff>

<commit_message>
2013-03-02 v2.0.56. Pushed a current version of the log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -17,13 +17,14 @@
     <sheet name="Organ Blood Flow" sheetId="7" r:id="rId8"/>
     <sheet name="Flows &amp; Conductances" sheetId="10" r:id="rId9"/>
     <sheet name="Cardiac Output" sheetId="13" r:id="rId10"/>
-    <sheet name="Osmoles" sheetId="19" r:id="rId11"/>
-    <sheet name="Blood Volume" sheetId="12" r:id="rId12"/>
-    <sheet name="Calories Used" sheetId="2" r:id="rId13"/>
-    <sheet name="Insulin Receptors" sheetId="14" r:id="rId14"/>
-    <sheet name="PV-Arteries" sheetId="15" r:id="rId15"/>
-    <sheet name="PV-Veins" sheetId="16" r:id="rId16"/>
-    <sheet name="PV-Lungs" sheetId="17" r:id="rId17"/>
+    <sheet name="Capys &amp; Lymph" sheetId="20" r:id="rId11"/>
+    <sheet name="Osmoles" sheetId="19" r:id="rId12"/>
+    <sheet name="Blood Volume" sheetId="12" r:id="rId13"/>
+    <sheet name="Calories Used" sheetId="2" r:id="rId14"/>
+    <sheet name="Insulin Receptors" sheetId="14" r:id="rId15"/>
+    <sheet name="PV-Arteries" sheetId="15" r:id="rId16"/>
+    <sheet name="PV-Veins" sheetId="16" r:id="rId17"/>
+    <sheet name="PV-Lungs" sheetId="17" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
@@ -91,6 +92,8 @@
     <definedName name="KidneyFlowMale">'Organ Blood Flow'!$C$16</definedName>
     <definedName name="KidneyMassFemale">'Organ Mass - Female'!$D$8</definedName>
     <definedName name="KidneyMassMale">'Organ Mass - Male'!$C$8</definedName>
+    <definedName name="L_P_K">'Capys &amp; Lymph'!$E$1</definedName>
+    <definedName name="L_P_Ratio">'Capys &amp; Lymph'!$E$1</definedName>
     <definedName name="LeftAtrialPressure">'Blood Pressures'!$B$18</definedName>
     <definedName name="LHeartFlowFemale">'Organ Blood Flow'!$H$27</definedName>
     <definedName name="LHeartFlowMale">'Organ Blood Flow'!$C$27</definedName>
@@ -219,6 +222,64 @@
     <author>Tom Coleman</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Coleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The target here is to have a lymph flow of 1.5 mL/Min and a L/P protein ratio of 0.7.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Coleman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[Lymph] = K*[Plasma + (1-K)*[Insterstitium]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tom Coleman</author>
+  </authors>
+  <commentList>
     <comment ref="B5" authorId="0">
       <text>
         <r>
@@ -250,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="282">
   <si>
     <t>Bone</t>
   </si>
@@ -1042,6 +1103,60 @@
   </si>
   <si>
     <t>Check Maht []</t>
+  </si>
+  <si>
+    <t>Capy's &amp; Lymph</t>
+  </si>
+  <si>
+    <t>Upper Torso</t>
+  </si>
+  <si>
+    <t>Middle Torso</t>
+  </si>
+  <si>
+    <t>Lower Torso</t>
+  </si>
+  <si>
+    <t>P-Capys</t>
+  </si>
+  <si>
+    <t>P-IFV</t>
+  </si>
+  <si>
+    <t>Cond</t>
+  </si>
+  <si>
+    <t>[Plasma]</t>
+  </si>
+  <si>
+    <t>[IFV]</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>H2O-Rate</t>
+  </si>
+  <si>
+    <t>Prot-Rate</t>
+  </si>
+  <si>
+    <t>Lymph</t>
+  </si>
+  <si>
+    <t>Fract</t>
+  </si>
+  <si>
+    <t>L/P K</t>
+  </si>
+  <si>
+    <t>[Lymph]</t>
+  </si>
+  <si>
+    <t>Plasma COP</t>
+  </si>
+  <si>
+    <t>IFV COP</t>
   </si>
 </sst>
 </file>
@@ -1815,10 +1930,318 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" t="s">
+        <v>273</v>
+      </c>
+      <c r="I3" t="s">
+        <v>275</v>
+      </c>
+      <c r="J3" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4">
+        <v>19.5</v>
+      </c>
+      <c r="C4">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="D4" s="3">
+        <f>E4/(B4-C4-F11+G11)</f>
+        <v>0.1130434782608697</v>
+      </c>
+      <c r="E4" s="6">
+        <f>J4</f>
+        <v>0.26</v>
+      </c>
+      <c r="F4">
+        <v>70</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4" s="7">
+        <f>I4/(F4-G4)</f>
+        <v>0.26</v>
+      </c>
+      <c r="I4" s="5">
+        <f>D11</f>
+        <v>13</v>
+      </c>
+      <c r="J4" s="6">
+        <f>K4*J7</f>
+        <v>0.26</v>
+      </c>
+      <c r="K4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5">
+        <v>19.5</v>
+      </c>
+      <c r="C5">
+        <v>-4.2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>E5/(B5-C5-F12+G12)</f>
+        <v>0.2571428571428574</v>
+      </c>
+      <c r="E5" s="6">
+        <f>J5</f>
+        <v>0.54</v>
+      </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5" s="7">
+        <f>I5/(F5-G5)</f>
+        <v>0.54</v>
+      </c>
+      <c r="I5" s="5">
+        <f>D12</f>
+        <v>27</v>
+      </c>
+      <c r="J5" s="6">
+        <f>K5*J7</f>
+        <v>0.54</v>
+      </c>
+      <c r="K5">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6">
+        <v>27.8</v>
+      </c>
+      <c r="C6">
+        <v>-4.2</v>
+      </c>
+      <c r="D6" s="3">
+        <f>E6/(B6-C6-F13+G13)</f>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="E6" s="6">
+        <f>J6</f>
+        <v>1.2</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" s="7">
+        <f>I6/(F6-G6)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I6" s="5">
+        <f>D13</f>
+        <v>60</v>
+      </c>
+      <c r="J6" s="6">
+        <f>K6*J7</f>
+        <v>1.2</v>
+      </c>
+      <c r="K6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6">
+        <f>J7</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="5">
+        <f>D14</f>
+        <v>100</v>
+      </c>
+      <c r="J7" s="6">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f>SUM(K4:K6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>275</v>
+      </c>
+      <c r="F10" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B11">
+        <f>L_P_K*F4+(1-L_P_K)*G4</f>
+        <v>50</v>
+      </c>
+      <c r="C11" s="6">
+        <f>E4</f>
+        <v>0.26</v>
+      </c>
+      <c r="D11">
+        <f>B11*C11</f>
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>28.1</v>
+      </c>
+      <c r="G11">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12">
+        <f>L_P_K*F5+(1-L_P_K)*G5</f>
+        <v>50</v>
+      </c>
+      <c r="C12" s="6">
+        <f>E5</f>
+        <v>0.54</v>
+      </c>
+      <c r="D12">
+        <f>B12*C12</f>
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <v>28.1</v>
+      </c>
+      <c r="G12">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13">
+        <f>L_P_K*F6+(1-L_P_K)*G6</f>
+        <v>50</v>
+      </c>
+      <c r="C13" s="6">
+        <f>E6</f>
+        <v>1.2</v>
+      </c>
+      <c r="D13">
+        <f>B13*C13</f>
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>28.1</v>
+      </c>
+      <c r="G13">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B11:B13)</f>
+        <v>150</v>
+      </c>
+      <c r="C14" s="6">
+        <f>E7</f>
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f>SUM(D11:D13)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1936,7 +2359,7 @@
         <v>2164.9402807200004</v>
       </c>
       <c r="E7" s="1">
-        <f>C7</f>
+        <f t="shared" ref="E7:E12" si="0">C7</f>
         <v>2164.9402807200004</v>
       </c>
     </row>
@@ -1952,7 +2375,7 @@
         <v>66.15095302200001</v>
       </c>
       <c r="E8" s="1">
-        <f>C8</f>
+        <f t="shared" si="0"/>
         <v>66.15095302200001</v>
       </c>
     </row>
@@ -1965,7 +2388,7 @@
         <v>2231.0912337420004</v>
       </c>
       <c r="E9" s="1">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>2231.0912337420004</v>
       </c>
     </row>
@@ -1978,7 +2401,7 @@
         <v>2231.0912337420004</v>
       </c>
       <c r="E10" s="1">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>2231.0912337420004</v>
       </c>
     </row>
@@ -1991,7 +2414,7 @@
         <v>4462.1824674840009</v>
       </c>
       <c r="E11" s="1">
-        <f>C11</f>
+        <f t="shared" si="0"/>
         <v>4462.1824674840009</v>
       </c>
     </row>
@@ -2004,7 +2427,7 @@
         <v>4149.8296947601211</v>
       </c>
       <c r="E12" s="1">
-        <f>C12</f>
+        <f t="shared" si="0"/>
         <v>4149.8296947601211</v>
       </c>
     </row>
@@ -2254,7 +2677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -2475,7 +2898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -2840,7 +3263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -3123,7 +3546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
@@ -4057,7 +4480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -5073,7 +5496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>

</xml_diff>

<commit_message>
2013-03-06 v2.0.57. Pushed a current version of the log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="6405" tabRatio="627" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -18,13 +18,12 @@
     <sheet name="Flows &amp; Conductances" sheetId="10" r:id="rId9"/>
     <sheet name="Cardiac Output" sheetId="13" r:id="rId10"/>
     <sheet name="Capys &amp; Lymph" sheetId="20" r:id="rId11"/>
-    <sheet name="Osmoles" sheetId="19" r:id="rId12"/>
-    <sheet name="Blood Volume" sheetId="12" r:id="rId13"/>
-    <sheet name="Calories Used" sheetId="2" r:id="rId14"/>
-    <sheet name="Insulin Receptors" sheetId="14" r:id="rId15"/>
-    <sheet name="PV-Arteries" sheetId="15" r:id="rId16"/>
-    <sheet name="PV-Veins" sheetId="16" r:id="rId17"/>
-    <sheet name="PV-Lungs" sheetId="17" r:id="rId18"/>
+    <sheet name="Blood Volume" sheetId="12" r:id="rId12"/>
+    <sheet name="Calories Used" sheetId="2" r:id="rId13"/>
+    <sheet name="Insulin Receptors" sheetId="14" r:id="rId14"/>
+    <sheet name="PV-Arteries" sheetId="15" r:id="rId15"/>
+    <sheet name="PV-Veins" sheetId="16" r:id="rId16"/>
+    <sheet name="PV-Lungs" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
@@ -311,7 +310,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="256">
   <si>
     <t>Bone</t>
   </si>
@@ -1012,15 +1011,6 @@
     <t>Rounded</t>
   </si>
   <si>
-    <t>Osmoles</t>
-  </si>
-  <si>
-    <t>ECFV</t>
-  </si>
-  <si>
-    <t>Dissociation</t>
-  </si>
-  <si>
     <t>H20 Mass</t>
   </si>
   <si>
@@ -1034,75 +1024,6 @@
   </si>
   <si>
     <t>Gut</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>External</t>
-  </si>
-  <si>
-    <t>[Osm]</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Receptor</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>Na+</t>
-  </si>
-  <si>
-    <t>K+</t>
-  </si>
-  <si>
-    <t>Total Anions</t>
-  </si>
-  <si>
-    <t>Total Cations</t>
-  </si>
-  <si>
-    <t>Total Ions</t>
-  </si>
-  <si>
-    <t>ECFV =========</t>
-  </si>
-  <si>
-    <t>Glucose</t>
-  </si>
-  <si>
-    <t>Urea</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Total Osmoles</t>
-  </si>
-  <si>
-    <t>Cell ==========</t>
-  </si>
-  <si>
-    <t>Check Math []</t>
-  </si>
-  <si>
-    <t>Total ! Ions</t>
-  </si>
-  <si>
-    <t>Active Ions</t>
-  </si>
-  <si>
-    <t>Total Active</t>
-  </si>
-  <si>
-    <t>Check Maht []</t>
   </si>
   <si>
     <t>Capy's &amp; Lymph</t>
@@ -1933,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1946,10 +1867,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="D1" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="E1">
         <v>0.6</v>
@@ -1957,39 +1878,39 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="C3" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="D3" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="E3" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="F3" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="G3" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="H3" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="I3" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="J3" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="K3" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="B4">
         <v>19.5</v>
@@ -2029,7 +1950,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <v>19.5</v>
@@ -2069,7 +1990,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="B6">
         <v>27.8</v>
@@ -2129,24 +2050,24 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
         <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="F10" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="G10" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="B11">
         <f>L_P_K*F4+(1-L_P_K)*G4</f>
@@ -2169,7 +2090,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="B12">
         <f>L_P_K*F5+(1-L_P_K)*G5</f>
@@ -2192,7 +2113,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="B13">
         <f>L_P_K*F6+(1-L_P_K)*G6</f>
@@ -2239,449 +2160,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2">
-        <v>0.93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>241</v>
-      </c>
-      <c r="H2" t="s">
-        <v>234</v>
-      </c>
-      <c r="I2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>302</v>
-      </c>
-      <c r="C3">
-        <v>282</v>
-      </c>
-      <c r="F3">
-        <f>Total_H2O</f>
-        <v>43019.367120000003</v>
-      </c>
-      <c r="G3">
-        <f>Cell_H2O</f>
-        <v>27010.059615000002</v>
-      </c>
-      <c r="H3">
-        <f>ECFV_H2O</f>
-        <v>15034.307505000001</v>
-      </c>
-      <c r="I3">
-        <f>External_H2O</f>
-        <v>975</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F4" s="5">
-        <f>F3/1000</f>
-        <v>43.019367120000005</v>
-      </c>
-      <c r="G4" s="5">
-        <f>G3/1000</f>
-        <v>27.010059615000003</v>
-      </c>
-      <c r="H4" s="5">
-        <f>H3/1000</f>
-        <v>15.034307505000001</v>
-      </c>
-      <c r="I4" s="5">
-        <f>I3/1000</f>
-        <v>0.97499999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>248</v>
-      </c>
-      <c r="B7">
-        <v>144</v>
-      </c>
-      <c r="C7" s="1">
-        <f>B7*H4</f>
-        <v>2164.9402807200004</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" ref="E7:E12" si="0">C7</f>
-        <v>2164.9402807200004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>249</v>
-      </c>
-      <c r="B8">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C8" s="1">
-        <f>B8*H4</f>
-        <v>66.15095302200001</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>66.15095302200001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>251</v>
-      </c>
-      <c r="C9" s="1">
-        <f>SUM(C7:C8)</f>
-        <v>2231.0912337420004</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>2231.0912337420004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" s="1">
-        <f>C9</f>
-        <v>2231.0912337420004</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>2231.0912337420004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>252</v>
-      </c>
-      <c r="C11" s="1">
-        <f>C9+C10</f>
-        <v>4462.1824674840009</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>4462.1824674840009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>261</v>
-      </c>
-      <c r="C12" s="1">
-        <f>E2*C11</f>
-        <v>4149.8296947601211</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>4149.8296947601211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>254</v>
-      </c>
-      <c r="B14">
-        <v>5.5</v>
-      </c>
-      <c r="C14" s="1">
-        <f>B14*H4</f>
-        <v>82.688691277499998</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>255</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1">
-        <f>B15*H4</f>
-        <v>60.137230020000004</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>256</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <f>C16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>260</v>
-      </c>
-      <c r="C17" s="1">
-        <f>SUM(C14:C16)</f>
-        <v>142.8259212975</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>257</v>
-      </c>
-      <c r="C19" s="1">
-        <f>SUM(C11,C17)</f>
-        <v>4605.0083887815008</v>
-      </c>
-      <c r="E19" s="1">
-        <f>SUM(E11,E17)</f>
-        <v>4462.1824674840009</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>259</v>
-      </c>
-      <c r="C20" s="1">
-        <f>C19/H4</f>
-        <v>306.3</v>
-      </c>
-      <c r="E20" s="1">
-        <f>E19/H4</f>
-        <v>296.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>262</v>
-      </c>
-      <c r="C22" s="1">
-        <f>SUM(C12,C17)</f>
-        <v>4292.655616057621</v>
-      </c>
-      <c r="E22" s="1">
-        <f>SUM(E12,E17)</f>
-        <v>4149.8296947601211</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>259</v>
-      </c>
-      <c r="C23" s="1">
-        <f>C22/H4</f>
-        <v>285.52400000000006</v>
-      </c>
-      <c r="E23" s="1">
-        <f>E22/H4</f>
-        <v>276.02400000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>249</v>
-      </c>
-      <c r="B27">
-        <v>140</v>
-      </c>
-      <c r="C27" s="1">
-        <f>B27*G4</f>
-        <v>3781.4083461000005</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>256</v>
-      </c>
-      <c r="B28">
-        <v>10</v>
-      </c>
-      <c r="C28" s="1">
-        <f>B28*G4</f>
-        <v>270.10059615</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>251</v>
-      </c>
-      <c r="C29" s="1">
-        <f>SUM(C27:C28)</f>
-        <v>4051.5089422500005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>250</v>
-      </c>
-      <c r="C30" s="1">
-        <f>C29</f>
-        <v>4051.5089422500005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>252</v>
-      </c>
-      <c r="C31" s="1">
-        <f>C29+C30</f>
-        <v>8103.0178845000009</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C32" s="1">
-        <f>E2*C31</f>
-        <v>7535.8066325850014</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>255</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1">
-        <f>B34*G4</f>
-        <v>108.04023846000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>256</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1">
-        <f>B35*G4</f>
-        <v>54.020119230000006</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>260</v>
-      </c>
-      <c r="C36" s="1">
-        <f>C34+C35</f>
-        <v>162.06035769000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>257</v>
-      </c>
-      <c r="C38" s="1">
-        <f>C31+C36</f>
-        <v>8265.0782421900003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>263</v>
-      </c>
-      <c r="C39">
-        <f>C38/G4</f>
-        <v>306</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>262</v>
-      </c>
-      <c r="C41" s="1">
-        <f>C32+C36</f>
-        <v>7697.8669902750016</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>259</v>
-      </c>
-      <c r="C42">
-        <f>C41/G4</f>
-        <v>285.00000000000006</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2898,7 +2379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -3263,7 +2744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -3546,7 +3027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
@@ -4480,7 +3961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -5496,7 +4977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -8342,7 +7823,7 @@
         <v>6525</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D27" s="1">
         <f>SUM(D20,D22,D24,D25,D26)</f>
@@ -8358,7 +7839,7 @@
         <v>75007.5</v>
       </c>
       <c r="C29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D29" s="1">
         <f>SUM(D16,D27)</f>
@@ -8367,7 +7848,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C31">
         <v>0.627</v>
@@ -8379,7 +7860,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C32">
         <f xml:space="preserve"> 0.349</f>
@@ -8392,7 +7873,7 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D33">
         <v>975</v>

</xml_diff>